<commit_message>
Cuaderno de estudio tema 6 de sexto y ajustes de escaleta
Cuaderno de estudio y escaleta
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion06/Escaleta_MA_06_06_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion06/Escaleta_MA_06_06_CO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8100" yWindow="3180" windowWidth="27920" windowHeight="15080"/>
+    <workbookView xWindow="10360" yWindow="20" windowWidth="27920" windowHeight="15080"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
@@ -13,7 +13,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$A$1:$U$2</definedName>
   </definedNames>
-  <calcPr calcId="140001" iterateCount="2" iterateDelta="10" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -404,9 +404,6 @@
     <t>La adición y la sustracción de fracciones</t>
   </si>
   <si>
-    <t>Soluciona problemas con adiciones y sustracciones con fracciones</t>
-  </si>
-  <si>
     <t>Practica la multiplicación y división de fracciones</t>
   </si>
   <si>
@@ -452,24 +449,15 @@
     <t>MT_07_06</t>
   </si>
   <si>
-    <t>Efectúa las sustracciones entre fracciones</t>
-  </si>
-  <si>
     <t>Soluciona problemas con sumas y restas de enteros y fracciones</t>
   </si>
   <si>
     <t xml:space="preserve">En la imagen de la izquierda colocar el enunciado en texto como imagen o una ilustración y a la derecha las alternativas de respuestas </t>
   </si>
   <si>
-    <t>Ejercicios para resolver problemas aplicando la adición o la sustracción de fracciones</t>
-  </si>
-  <si>
     <t>Completa las tablas de sumas y restas de fracciones</t>
   </si>
   <si>
-    <t>Ejercicios de razonamiento para reforzar las operaciones de adición y sustracción de fracciones</t>
-  </si>
-  <si>
     <t>En la imagen a la izquierda dar  cuadros mágicos, de tal manera que las sumas en todas las direcciones sea la misma. En las opciones de respuestas las dos o tres fracciones que falten para completar la tabla. Pueden estar las tres en una sola imagen o una en cada espacio de respuesta.</t>
   </si>
   <si>
@@ -527,9 +515,6 @@
     <t>La multiplicación de fracciones</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje:Polinomios aritméticos con fracciones</t>
-  </si>
-  <si>
     <t>Competencias</t>
   </si>
   <si>
@@ -542,9 +527,6 @@
     <t>Actividades sobre La adición y la sustracción de fracciones</t>
   </si>
   <si>
-    <t>Ejercicios para practicar la multiplicación y división de fracciones</t>
-  </si>
-  <si>
     <t>Actividad para resolver problemas con fracciones</t>
   </si>
   <si>
@@ -557,9 +539,6 @@
     <t>Actividad para practicar las operaciones combinadas con fracciones</t>
   </si>
   <si>
-    <t>Ejercicios para reforzar los algoritmos de las operaciones con fracciones</t>
-  </si>
-  <si>
     <t>Actividad para organizar el proceso para resolver operaciones combinadas</t>
   </si>
   <si>
@@ -572,30 +551,15 @@
     <t>Actividades sobre Los polinomios ariméticos</t>
   </si>
   <si>
-    <t>Actividad que propone realizar el desarrollo de las destrezas para resolver una operación combinada</t>
-  </si>
-  <si>
-    <t>Actividad que propone realizar el procedimiento para determinar el resultado de una multiplicación</t>
-  </si>
-  <si>
     <t>Mapa conceptual sobre el tema Las operaciones con fracciones</t>
   </si>
   <si>
     <t>Evalúa tus conocimientos sobre el tema Las operaciones con fracciones</t>
   </si>
   <si>
-    <t>Actividad para aplicar el algoritmo de la adición de fracciones</t>
-  </si>
-  <si>
-    <t>Actividad para aplicar el algoritmo de la sustracción de fracciones</t>
-  </si>
-  <si>
     <t>Actividad para aplicar el algoritmo de la multiplicación de fracciones</t>
   </si>
   <si>
-    <t>Ejercicios para aplicar la multiplicación de fracciones</t>
-  </si>
-  <si>
     <t>Actividades sobre La multiplicación de fracciones</t>
   </si>
   <si>
@@ -690,6 +654,42 @@
   </si>
   <si>
     <t>Actividad para plantear y resolver situaciones con fracciones</t>
+  </si>
+  <si>
+    <t>Efectúa operaciones entre fracciones</t>
+  </si>
+  <si>
+    <t>Actividad para aplicar los algoritmos de adición y sustracción</t>
+  </si>
+  <si>
+    <t>Actividad para resolver operaciones entre fracciones</t>
+  </si>
+  <si>
+    <t>Actividad para resolver operaciones combinadas de adiciones y sustracciones</t>
+  </si>
+  <si>
+    <t>Soluciona problemas de adición y sustracción entre fracciones</t>
+  </si>
+  <si>
+    <t>Actividad para resolver problemas aplicando la adición o la sustracción de fracciones</t>
+  </si>
+  <si>
+    <t>Actividades para aplicar la multiplicación de fracciones</t>
+  </si>
+  <si>
+    <t>Actividades para practicar la multiplicación y división de fracciones</t>
+  </si>
+  <si>
+    <t>Actividades para reforzar los algoritmos de las operaciones con fracciones</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: Los polinomios aritméticos con fracciones</t>
+  </si>
+  <si>
+    <t>Actividad para resolver una operación combinada</t>
+  </si>
+  <si>
+    <t>Actividad que propone estrategias para multiplicar</t>
   </si>
 </sst>
 </file>
@@ -1027,31 +1027,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1091,6 +1076,21 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1404,9 +1404,9 @@
   <sheetPr codeName="Hoja1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:U295"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J33" sqref="J33"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1434,104 +1434,104 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="23" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="65" t="s">
+      <c r="C1" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="56" t="s">
+      <c r="D1" s="51" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="54" t="s">
+      <c r="E1" s="49" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="52" t="s">
+      <c r="F1" s="45" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="58" t="s">
+      <c r="G1" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="52" t="s">
+      <c r="H1" s="45" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="52" t="s">
+      <c r="I1" s="45" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="62" t="s">
+      <c r="J1" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="60" t="s">
+      <c r="K1" s="55" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="58" t="s">
+      <c r="L1" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="64" t="s">
+      <c r="M1" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="64"/>
-      <c r="O1" s="45" t="s">
+      <c r="N1" s="59"/>
+      <c r="O1" s="47" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="45" t="s">
+      <c r="P1" s="47" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="47" t="s">
+      <c r="Q1" s="62" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="50" t="s">
+      <c r="R1" s="65" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="47" t="s">
+      <c r="S1" s="62" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="49" t="s">
+      <c r="T1" s="64" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="47" t="s">
+      <c r="U1" s="62" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="23" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A2" s="57"/>
-      <c r="B2" s="55"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="63"/>
-      <c r="K2" s="61"/>
-      <c r="L2" s="59"/>
+      <c r="A2" s="52"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="54"/>
       <c r="M2" s="24" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
-      <c r="Q2" s="48"/>
-      <c r="R2" s="51"/>
-      <c r="S2" s="48"/>
-      <c r="T2" s="49"/>
-      <c r="U2" s="48"/>
+      <c r="O2" s="48"/>
+      <c r="P2" s="48"/>
+      <c r="Q2" s="63"/>
+      <c r="R2" s="66"/>
+      <c r="S2" s="63"/>
+      <c r="T2" s="64"/>
+      <c r="U2" s="63"/>
     </row>
     <row r="3" spans="1:21" ht="16" thickTop="1">
       <c r="A3" s="15" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D3" s="15" t="s">
         <v>125</v>
@@ -1548,7 +1548,7 @@
         <v>19</v>
       </c>
       <c r="J3" s="20" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K3" s="21" t="s">
         <v>19</v>
@@ -1559,7 +1559,7 @@
       <c r="M3" s="22"/>
       <c r="N3" s="22"/>
       <c r="O3" s="33" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="P3" s="34" t="s">
         <v>19</v>
@@ -1568,16 +1568,16 @@
         <v>7</v>
       </c>
       <c r="R3" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="S3" s="35" t="s">
         <v>138</v>
       </c>
-      <c r="S3" s="35" t="s">
+      <c r="T3" s="37" t="s">
         <v>139</v>
       </c>
-      <c r="T3" s="37" t="s">
+      <c r="U3" s="35" t="s">
         <v>140</v>
-      </c>
-      <c r="U3" s="35" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15">
@@ -1585,10 +1585,10 @@
         <v>15</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D4" s="15" t="s">
         <v>125</v>
@@ -1596,7 +1596,7 @@
       <c r="E4" s="16"/>
       <c r="F4" s="18"/>
       <c r="G4" s="26" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="H4" s="18">
         <v>2</v>
@@ -1605,7 +1605,7 @@
         <v>20</v>
       </c>
       <c r="J4" s="20" t="s">
-        <v>186</v>
+        <v>211</v>
       </c>
       <c r="K4" s="21" t="s">
         <v>20</v>
@@ -1616,7 +1616,7 @@
       <c r="M4" s="22"/>
       <c r="N4" s="22"/>
       <c r="O4" s="33" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="P4" s="34" t="s">
         <v>19</v>
@@ -1625,16 +1625,16 @@
         <v>6</v>
       </c>
       <c r="R4" s="36" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="S4" s="35" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="T4" s="38" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="U4" s="35" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15">
@@ -1642,10 +1642,10 @@
         <v>15</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>125</v>
@@ -1653,7 +1653,7 @@
       <c r="E5" s="16"/>
       <c r="F5" s="18"/>
       <c r="G5" s="26" t="s">
-        <v>142</v>
+        <v>210</v>
       </c>
       <c r="H5" s="18">
         <v>3</v>
@@ -1662,7 +1662,7 @@
         <v>20</v>
       </c>
       <c r="J5" s="20" t="s">
-        <v>187</v>
+        <v>212</v>
       </c>
       <c r="K5" s="21" t="s">
         <v>20</v>
@@ -1673,7 +1673,7 @@
       <c r="M5" s="22"/>
       <c r="N5" s="22"/>
       <c r="O5" s="33" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="P5" s="34" t="s">
         <v>19</v>
@@ -1682,16 +1682,16 @@
         <v>6</v>
       </c>
       <c r="R5" s="36" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="S5" s="35" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="T5" s="38" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="U5" s="35" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="15">
@@ -1699,10 +1699,10 @@
         <v>15</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D6" s="15" t="s">
         <v>125</v>
@@ -1710,7 +1710,7 @@
       <c r="E6" s="39"/>
       <c r="F6" s="40"/>
       <c r="G6" s="26" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="H6" s="18">
         <v>4</v>
@@ -1719,7 +1719,7 @@
         <v>20</v>
       </c>
       <c r="J6" s="41" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="K6" s="21" t="s">
         <v>19</v>
@@ -1737,16 +1737,16 @@
         <v>7</v>
       </c>
       <c r="R6" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="S6" s="35" t="s">
         <v>138</v>
       </c>
-      <c r="S6" s="35" t="s">
-        <v>139</v>
-      </c>
       <c r="T6" s="37" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="U6" s="35" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="15">
@@ -1754,10 +1754,10 @@
         <v>15</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D7" s="15" t="s">
         <v>125</v>
@@ -1765,7 +1765,7 @@
       <c r="E7" s="39"/>
       <c r="F7" s="40"/>
       <c r="G7" s="26" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H7" s="18">
         <v>5</v>
@@ -1774,7 +1774,7 @@
         <v>20</v>
       </c>
       <c r="J7" s="41" t="s">
-        <v>147</v>
+        <v>213</v>
       </c>
       <c r="K7" s="21" t="s">
         <v>20</v>
@@ -1787,7 +1787,7 @@
         <v>39</v>
       </c>
       <c r="O7" s="40" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="P7" s="34" t="s">
         <v>20</v>
@@ -1796,16 +1796,16 @@
         <v>6</v>
       </c>
       <c r="R7" s="36" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="S7" s="35" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="T7" s="42" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="U7" s="35" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="15">
@@ -1813,10 +1813,10 @@
         <v>15</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D8" s="15" t="s">
         <v>125</v>
@@ -1824,7 +1824,7 @@
       <c r="E8" s="39"/>
       <c r="F8" s="40"/>
       <c r="G8" s="26" t="s">
-        <v>126</v>
+        <v>214</v>
       </c>
       <c r="H8" s="18">
         <v>6</v>
@@ -1833,7 +1833,7 @@
         <v>20</v>
       </c>
       <c r="J8" s="41" t="s">
-        <v>145</v>
+        <v>215</v>
       </c>
       <c r="K8" s="21" t="s">
         <v>20</v>
@@ -1846,7 +1846,7 @@
         <v>39</v>
       </c>
       <c r="O8" s="40" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="P8" s="34" t="s">
         <v>19</v>
@@ -1855,16 +1855,16 @@
         <v>6</v>
       </c>
       <c r="R8" s="36" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="S8" s="35" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="T8" s="42" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="U8" s="35" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="15">
@@ -1872,10 +1872,10 @@
         <v>15</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D9" s="15" t="s">
         <v>125</v>
@@ -1885,7 +1885,7 @@
       </c>
       <c r="F9" s="40"/>
       <c r="G9" s="26" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="H9" s="18">
         <v>7</v>
@@ -1894,7 +1894,7 @@
         <v>20</v>
       </c>
       <c r="J9" s="41" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="K9" s="21" t="s">
         <v>19</v>
@@ -1912,16 +1912,16 @@
         <v>7</v>
       </c>
       <c r="R9" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="S9" s="35" t="s">
         <v>138</v>
       </c>
-      <c r="S9" s="35" t="s">
-        <v>139</v>
-      </c>
       <c r="T9" s="37" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="U9" s="35" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:21" ht="15">
@@ -1929,18 +1929,18 @@
         <v>15</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="E10" s="39"/>
       <c r="F10" s="40"/>
       <c r="G10" s="26" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="H10" s="18">
         <v>8</v>
@@ -1949,7 +1949,7 @@
         <v>20</v>
       </c>
       <c r="J10" s="20" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="K10" s="21" t="s">
         <v>20</v>
@@ -1960,7 +1960,7 @@
       <c r="M10" s="8"/>
       <c r="N10" s="8"/>
       <c r="O10" s="40" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="P10" s="34" t="s">
         <v>19</v>
@@ -1969,16 +1969,16 @@
         <v>6</v>
       </c>
       <c r="R10" s="36" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="S10" s="35" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="T10" s="38" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="U10" s="35" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="15">
@@ -1986,18 +1986,18 @@
         <v>15</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="E11" s="39"/>
       <c r="F11" s="40"/>
       <c r="G11" s="26" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="H11" s="18">
         <v>9</v>
@@ -2006,7 +2006,7 @@
         <v>20</v>
       </c>
       <c r="J11" s="41" t="s">
-        <v>189</v>
+        <v>216</v>
       </c>
       <c r="K11" s="21" t="s">
         <v>20</v>
@@ -2019,7 +2019,7 @@
         <v>33</v>
       </c>
       <c r="O11" s="40" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="P11" s="34" t="s">
         <v>19</v>
@@ -2028,16 +2028,16 @@
         <v>6</v>
       </c>
       <c r="R11" s="36" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="S11" s="35" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="T11" s="42" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="U11" s="35" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="15">
@@ -2045,20 +2045,20 @@
         <v>15</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="E12" s="39" t="s">
         <v>124</v>
       </c>
       <c r="F12" s="40"/>
       <c r="G12" s="26" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="H12" s="18">
         <v>10</v>
@@ -2067,7 +2067,7 @@
         <v>20</v>
       </c>
       <c r="J12" s="41" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="K12" s="21" t="s">
         <v>20</v>
@@ -2085,16 +2085,16 @@
         <v>7</v>
       </c>
       <c r="R12" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="S12" s="35" t="s">
         <v>138</v>
       </c>
-      <c r="S12" s="35" t="s">
-        <v>139</v>
-      </c>
       <c r="T12" s="37" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="U12" s="35" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="15">
@@ -2102,18 +2102,18 @@
         <v>15</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="E13" s="39"/>
       <c r="F13" s="40"/>
       <c r="G13" s="26" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="H13" s="18">
         <v>11</v>
@@ -2122,7 +2122,7 @@
         <v>20</v>
       </c>
       <c r="J13" s="20" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="K13" s="21" t="s">
         <v>20</v>
@@ -2133,7 +2133,7 @@
       <c r="M13" s="8"/>
       <c r="N13" s="8"/>
       <c r="O13" s="40" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="P13" s="34" t="s">
         <v>19</v>
@@ -2142,16 +2142,16 @@
         <v>6</v>
       </c>
       <c r="R13" s="36" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="S13" s="35" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="T13" s="38" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="U13" s="35" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="15">
@@ -2159,18 +2159,18 @@
         <v>15</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="E14" s="39"/>
       <c r="F14" s="40"/>
       <c r="G14" s="26" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="H14" s="18">
         <v>12</v>
@@ -2179,7 +2179,7 @@
         <v>19</v>
       </c>
       <c r="J14" s="41" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="K14" s="21" t="s">
         <v>19</v>
@@ -2197,16 +2197,16 @@
         <v>7</v>
       </c>
       <c r="R14" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="S14" s="35" t="s">
         <v>138</v>
       </c>
-      <c r="S14" s="35" t="s">
-        <v>139</v>
-      </c>
       <c r="T14" s="37" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="U14" s="35" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="15">
@@ -2214,18 +2214,18 @@
         <v>15</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="E15" s="39"/>
       <c r="F15" s="40"/>
       <c r="G15" s="26" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H15" s="18">
         <v>13</v>
@@ -2234,7 +2234,7 @@
         <v>20</v>
       </c>
       <c r="J15" s="41" t="s">
-        <v>172</v>
+        <v>217</v>
       </c>
       <c r="K15" s="21" t="s">
         <v>19</v>
@@ -2252,16 +2252,16 @@
         <v>7</v>
       </c>
       <c r="R15" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="S15" s="35" t="s">
         <v>138</v>
       </c>
-      <c r="S15" s="35" t="s">
-        <v>139</v>
-      </c>
       <c r="T15" s="37" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="U15" s="35" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="15">
@@ -2269,18 +2269,18 @@
         <v>15</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="E16" s="39"/>
       <c r="F16" s="40"/>
       <c r="G16" s="26" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="H16" s="18">
         <v>14</v>
@@ -2289,7 +2289,7 @@
         <v>20</v>
       </c>
       <c r="J16" s="41" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="K16" s="21" t="s">
         <v>20</v>
@@ -2302,7 +2302,7 @@
         <v>29</v>
       </c>
       <c r="O16" s="40" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="P16" s="43" t="s">
         <v>20</v>
@@ -2311,16 +2311,16 @@
         <v>6</v>
       </c>
       <c r="R16" s="36" t="s">
+        <v>183</v>
+      </c>
+      <c r="S16" s="35" t="s">
+        <v>188</v>
+      </c>
+      <c r="T16" s="42" t="s">
         <v>195</v>
       </c>
-      <c r="S16" s="35" t="s">
-        <v>200</v>
-      </c>
-      <c r="T16" s="42" t="s">
-        <v>207</v>
-      </c>
       <c r="U16" s="35" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="15">
@@ -2328,13 +2328,13 @@
         <v>15</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="E17" s="39"/>
       <c r="F17" s="40"/>
@@ -2348,7 +2348,7 @@
         <v>20</v>
       </c>
       <c r="J17" s="41" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="K17" s="21" t="s">
         <v>19</v>
@@ -2366,16 +2366,16 @@
         <v>7</v>
       </c>
       <c r="R17" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="S17" s="35" t="s">
         <v>138</v>
-      </c>
-      <c r="S17" s="35" t="s">
-        <v>139</v>
       </c>
       <c r="T17" s="37" t="s">
         <v>122</v>
       </c>
       <c r="U17" s="35" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="15">
@@ -2383,20 +2383,20 @@
         <v>15</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="E18" s="39" t="s">
         <v>124</v>
       </c>
       <c r="F18" s="40"/>
       <c r="G18" s="26" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="H18" s="18">
         <v>16</v>
@@ -2405,7 +2405,7 @@
         <v>20</v>
       </c>
       <c r="J18" s="41" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="K18" s="21" t="s">
         <v>19</v>
@@ -2423,16 +2423,16 @@
         <v>7</v>
       </c>
       <c r="R18" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="S18" s="35" t="s">
         <v>138</v>
       </c>
-      <c r="S18" s="35" t="s">
-        <v>139</v>
-      </c>
       <c r="T18" s="37" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="U18" s="35" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="19" spans="1:21" ht="15">
@@ -2440,18 +2440,18 @@
         <v>15</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="E19" s="39"/>
       <c r="F19" s="40"/>
       <c r="G19" s="26" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H19" s="18">
         <v>17</v>
@@ -2460,7 +2460,7 @@
         <v>20</v>
       </c>
       <c r="J19" s="41" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="K19" s="21" t="s">
         <v>19</v>
@@ -2478,16 +2478,16 @@
         <v>7</v>
       </c>
       <c r="R19" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="S19" s="35" t="s">
         <v>138</v>
       </c>
-      <c r="S19" s="35" t="s">
-        <v>139</v>
-      </c>
       <c r="T19" s="37" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="U19" s="35" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="20" spans="1:21" ht="15">
@@ -2495,18 +2495,18 @@
         <v>15</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="E20" s="39"/>
       <c r="F20" s="40"/>
       <c r="G20" s="26" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H20" s="18">
         <v>18</v>
@@ -2515,7 +2515,7 @@
         <v>19</v>
       </c>
       <c r="J20" s="41" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="K20" s="21" t="s">
         <v>20</v>
@@ -2533,16 +2533,16 @@
         <v>7</v>
       </c>
       <c r="R20" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="S20" s="35" t="s">
         <v>138</v>
       </c>
-      <c r="S20" s="35" t="s">
-        <v>139</v>
-      </c>
       <c r="T20" s="37" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="U20" s="35" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="21" spans="1:21" ht="15" customHeight="1">
@@ -2550,18 +2550,18 @@
         <v>15</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="E21" s="39"/>
       <c r="F21" s="40"/>
       <c r="G21" s="26" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="H21" s="18">
         <v>19</v>
@@ -2570,7 +2570,7 @@
         <v>20</v>
       </c>
       <c r="J21" s="41" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="K21" s="21" t="s">
         <v>19</v>
@@ -2583,7 +2583,7 @@
         <v>39</v>
       </c>
       <c r="O21" s="40" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="P21" s="43" t="s">
         <v>20</v>
@@ -2592,16 +2592,16 @@
         <v>6</v>
       </c>
       <c r="R21" s="36" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="S21" s="35" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="T21" s="42" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="U21" s="35" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
     </row>
     <row r="22" spans="1:21" ht="15">
@@ -2609,18 +2609,18 @@
         <v>15</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="E22" s="39"/>
       <c r="F22" s="40"/>
       <c r="G22" s="26" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H22" s="18">
         <v>20</v>
@@ -2629,7 +2629,7 @@
         <v>20</v>
       </c>
       <c r="J22" s="41" t="s">
-        <v>177</v>
+        <v>218</v>
       </c>
       <c r="K22" s="21" t="s">
         <v>19</v>
@@ -2647,16 +2647,16 @@
         <v>7</v>
       </c>
       <c r="R22" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="S22" s="35" t="s">
         <v>138</v>
       </c>
-      <c r="S22" s="35" t="s">
-        <v>139</v>
-      </c>
       <c r="T22" s="37" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="U22" s="35" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="23" spans="1:21" ht="15">
@@ -2664,18 +2664,18 @@
         <v>15</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="E23" s="39"/>
       <c r="F23" s="40"/>
       <c r="G23" s="26" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H23" s="18">
         <v>21</v>
@@ -2684,7 +2684,7 @@
         <v>20</v>
       </c>
       <c r="J23" s="41" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="K23" s="21" t="s">
         <v>19</v>
@@ -2702,16 +2702,16 @@
         <v>7</v>
       </c>
       <c r="R23" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="S23" s="35" t="s">
         <v>138</v>
       </c>
-      <c r="S23" s="35" t="s">
-        <v>139</v>
-      </c>
       <c r="T23" s="37" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="U23" s="35" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="15">
@@ -2719,18 +2719,18 @@
         <v>15</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="E24" s="39"/>
       <c r="F24" s="40"/>
       <c r="G24" s="26" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="H24" s="18">
         <v>22</v>
@@ -2739,7 +2739,7 @@
         <v>20</v>
       </c>
       <c r="J24" s="41" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="K24" s="21" t="s">
         <v>19</v>
@@ -2757,16 +2757,16 @@
         <v>7</v>
       </c>
       <c r="R24" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="S24" s="35" t="s">
         <v>138</v>
       </c>
-      <c r="S24" s="35" t="s">
-        <v>139</v>
-      </c>
       <c r="T24" s="37" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="U24" s="35" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="25" spans="1:21" ht="15">
@@ -2774,18 +2774,18 @@
         <v>15</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="E25" s="39"/>
       <c r="F25" s="40"/>
       <c r="G25" s="26" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H25" s="18">
         <v>23</v>
@@ -2794,7 +2794,7 @@
         <v>19</v>
       </c>
       <c r="J25" s="41" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="K25" s="21" t="s">
         <v>19</v>
@@ -2812,16 +2812,16 @@
         <v>7</v>
       </c>
       <c r="R25" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="S25" s="35" t="s">
         <v>138</v>
       </c>
-      <c r="S25" s="35" t="s">
-        <v>139</v>
-      </c>
       <c r="T25" s="37" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="U25" s="35" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="26" spans="1:21" ht="15">
@@ -2829,20 +2829,20 @@
         <v>15</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="E26" s="39" t="s">
         <v>124</v>
       </c>
       <c r="F26" s="40"/>
       <c r="G26" s="26" t="s">
-        <v>167</v>
+        <v>219</v>
       </c>
       <c r="H26" s="18">
         <v>24</v>
@@ -2851,7 +2851,7 @@
         <v>20</v>
       </c>
       <c r="J26" s="41" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="K26" s="21" t="s">
         <v>19</v>
@@ -2869,16 +2869,16 @@
         <v>7</v>
       </c>
       <c r="R26" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="S26" s="35" t="s">
         <v>138</v>
       </c>
-      <c r="S26" s="35" t="s">
-        <v>139</v>
-      </c>
       <c r="T26" s="37" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="U26" s="35" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="27" spans="1:21" ht="15">
@@ -2886,18 +2886,18 @@
         <v>15</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D27" s="44" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="E27" s="39"/>
       <c r="F27" s="40"/>
       <c r="G27" s="26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H27" s="18">
         <v>25</v>
@@ -2906,7 +2906,7 @@
         <v>20</v>
       </c>
       <c r="J27" s="41" t="s">
-        <v>182</v>
+        <v>220</v>
       </c>
       <c r="K27" s="21" t="s">
         <v>19</v>
@@ -2924,16 +2924,16 @@
         <v>7</v>
       </c>
       <c r="R27" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="S27" s="35" t="s">
         <v>138</v>
       </c>
-      <c r="S27" s="35" t="s">
-        <v>139</v>
-      </c>
       <c r="T27" s="37" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="U27" s="35" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="28" spans="1:21" ht="15">
@@ -2941,18 +2941,18 @@
         <v>15</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D28" s="44" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="E28" s="39"/>
       <c r="F28" s="40"/>
       <c r="G28" s="26" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="H28" s="18">
         <v>26</v>
@@ -2961,7 +2961,7 @@
         <v>20</v>
       </c>
       <c r="J28" s="41" t="s">
-        <v>183</v>
+        <v>221</v>
       </c>
       <c r="K28" s="21" t="s">
         <v>19</v>
@@ -2979,16 +2979,16 @@
         <v>7</v>
       </c>
       <c r="R28" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="S28" s="35" t="s">
         <v>138</v>
       </c>
-      <c r="S28" s="35" t="s">
-        <v>139</v>
-      </c>
       <c r="T28" s="37" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="U28" s="35" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="29" spans="1:21" ht="15">
@@ -2996,13 +2996,13 @@
         <v>15</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D29" s="44" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="E29" s="39"/>
       <c r="F29" s="40"/>
@@ -3016,7 +3016,7 @@
         <v>20</v>
       </c>
       <c r="J29" s="41" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="K29" s="21" t="s">
         <v>20</v>
@@ -3041,13 +3041,13 @@
         <v>15</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D30" s="44" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="E30" s="39"/>
       <c r="F30" s="40"/>
@@ -3061,7 +3061,7 @@
         <v>20</v>
       </c>
       <c r="J30" s="41" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="K30" s="21" t="s">
         <v>20</v>
@@ -3074,7 +3074,7 @@
         <v>33</v>
       </c>
       <c r="O30" s="40" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="P30" s="43" t="s">
         <v>19</v>
@@ -3083,16 +3083,16 @@
         <v>6</v>
       </c>
       <c r="R30" s="36" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="S30" s="35" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="T30" s="42" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="U30" s="35" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
     </row>
     <row r="31" spans="1:21" ht="15">
@@ -3100,18 +3100,18 @@
         <v>15</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D31" s="44" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="E31" s="39"/>
       <c r="F31" s="40"/>
       <c r="G31" s="44" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="H31" s="18">
         <v>29</v>
@@ -3129,7 +3129,7 @@
         <v>52</v>
       </c>
       <c r="O31" s="40" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="P31" s="43" t="s">
         <v>20</v>
@@ -3138,16 +3138,16 @@
         <v>6</v>
       </c>
       <c r="R31" s="36" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="S31" s="35" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="T31" s="37" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="U31" s="35" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
     </row>
     <row r="32" spans="1:21" ht="15">
@@ -4660,6 +4660,12 @@
     <row r="295" hidden="1"/>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4674,15 +4680,8 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">

</xml_diff>

<commit_message>
Ajustes de título de nombre
Ajustes de nombre de recurso
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion06/Escaleta_MA_06_06_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion06/Escaleta_MA_06_06_CO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10360" yWindow="20" windowWidth="27920" windowHeight="15080"/>
+    <workbookView xWindow="2860" yWindow="260" windowWidth="27920" windowHeight="15080"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
@@ -455,9 +455,6 @@
     <t xml:space="preserve">En la imagen de la izquierda colocar el enunciado en texto como imagen o una ilustración y a la derecha las alternativas de respuestas </t>
   </si>
   <si>
-    <t>Completa las tablas de sumas y restas de fracciones</t>
-  </si>
-  <si>
     <t>En la imagen a la izquierda dar  cuadros mágicos, de tal manera que las sumas en todas las direcciones sea la misma. En las opciones de respuestas las dos o tres fracciones que falten para completar la tabla. Pueden estar las tres en una sola imagen o una en cada espacio de respuesta.</t>
   </si>
   <si>
@@ -690,6 +687,9 @@
   </si>
   <si>
     <t>Actividad que propone estrategias para multiplicar</t>
+  </si>
+  <si>
+    <t>Completa tablas de sumas y restas de fracciones</t>
   </si>
 </sst>
 </file>
@@ -916,14 +916,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -962,9 +970,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1027,16 +1032,31 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1078,27 +1098,26 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="13">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1404,9 +1423,9 @@
   <sheetPr codeName="Hoja1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:U295"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J28" sqref="J28"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1420,108 +1439,108 @@
     <col min="7" max="7" width="51.33203125" customWidth="1"/>
     <col min="8" max="8" width="12.33203125" style="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="1" customWidth="1"/>
-    <col min="10" max="10" width="73.5" customWidth="1"/>
+    <col min="10" max="10" width="82.5" customWidth="1"/>
     <col min="11" max="11" width="13.33203125" customWidth="1"/>
     <col min="12" max="12" width="17.5" customWidth="1"/>
     <col min="13" max="14" width="9.33203125" customWidth="1"/>
     <col min="15" max="15" width="58.5" style="1" customWidth="1"/>
-    <col min="16" max="16" width="16.5" style="31" customWidth="1"/>
-    <col min="17" max="17" width="20.5" style="31" customWidth="1"/>
-    <col min="18" max="18" width="23" style="27" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="20.6640625" style="27" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="25.83203125" style="27" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="21.6640625" style="27" customWidth="1"/>
+    <col min="16" max="16" width="16.5" style="30" customWidth="1"/>
+    <col min="17" max="17" width="20.5" style="30" customWidth="1"/>
+    <col min="18" max="18" width="23" style="26" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.6640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="25.83203125" style="26" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="21.6640625" style="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="23" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A1" s="51" t="s">
+    <row r="1" spans="1:21" s="22" customFormat="1" ht="33.75" customHeight="1">
+      <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="60" t="s">
+      <c r="C1" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="55" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="49" t="s">
+      <c r="E1" s="53" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="45" t="s">
+      <c r="F1" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="53" t="s">
+      <c r="G1" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="45" t="s">
+      <c r="H1" s="51" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="45" t="s">
+      <c r="I1" s="51" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="57" t="s">
+      <c r="J1" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="55" t="s">
+      <c r="K1" s="59" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="53" t="s">
+      <c r="L1" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="59" t="s">
+      <c r="M1" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="59"/>
-      <c r="O1" s="47" t="s">
+      <c r="N1" s="63"/>
+      <c r="O1" s="44" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="47" t="s">
+      <c r="P1" s="44" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="62" t="s">
+      <c r="Q1" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="65" t="s">
+      <c r="R1" s="49" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="62" t="s">
+      <c r="S1" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="64" t="s">
+      <c r="T1" s="48" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="62" t="s">
+      <c r="U1" s="46" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="23" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A2" s="52"/>
-      <c r="B2" s="50"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="58"/>
-      <c r="K2" s="56"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="24" t="s">
+    <row r="2" spans="1:21" s="22" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A2" s="56"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="60"/>
+      <c r="L2" s="58"/>
+      <c r="M2" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="N2" s="24" t="s">
+      <c r="N2" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="48"/>
-      <c r="P2" s="48"/>
-      <c r="Q2" s="63"/>
-      <c r="R2" s="66"/>
-      <c r="S2" s="63"/>
-      <c r="T2" s="64"/>
-      <c r="U2" s="63"/>
+      <c r="O2" s="45"/>
+      <c r="P2" s="45"/>
+      <c r="Q2" s="47"/>
+      <c r="R2" s="50"/>
+      <c r="S2" s="47"/>
+      <c r="T2" s="48"/>
+      <c r="U2" s="47"/>
     </row>
     <row r="3" spans="1:21" ht="16" thickTop="1">
       <c r="A3" s="15" t="s">
@@ -1538,7 +1557,7 @@
       </c>
       <c r="E3" s="16"/>
       <c r="F3" s="18"/>
-      <c r="G3" s="26" t="s">
+      <c r="G3" s="25" t="s">
         <v>125</v>
       </c>
       <c r="H3" s="18">
@@ -1547,36 +1566,36 @@
       <c r="I3" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="20" t="s">
+      <c r="J3" s="66" t="s">
         <v>136</v>
       </c>
-      <c r="K3" s="21" t="s">
+      <c r="K3" s="20" t="s">
         <v>19</v>
       </c>
       <c r="L3" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="22"/>
-      <c r="N3" s="22"/>
-      <c r="O3" s="33" t="s">
-        <v>201</v>
-      </c>
-      <c r="P3" s="34" t="s">
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="32" t="s">
+        <v>200</v>
+      </c>
+      <c r="P3" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="Q3" s="35">
+      <c r="Q3" s="34">
         <v>7</v>
       </c>
-      <c r="R3" s="36" t="s">
+      <c r="R3" s="35" t="s">
         <v>137</v>
       </c>
-      <c r="S3" s="35" t="s">
+      <c r="S3" s="34" t="s">
         <v>138</v>
       </c>
-      <c r="T3" s="37" t="s">
+      <c r="T3" s="36" t="s">
         <v>139</v>
       </c>
-      <c r="U3" s="35" t="s">
+      <c r="U3" s="34" t="s">
         <v>140</v>
       </c>
     </row>
@@ -1595,8 +1614,8 @@
       </c>
       <c r="E4" s="16"/>
       <c r="F4" s="18"/>
-      <c r="G4" s="26" t="s">
-        <v>204</v>
+      <c r="G4" s="25" t="s">
+        <v>203</v>
       </c>
       <c r="H4" s="18">
         <v>2</v>
@@ -1604,37 +1623,37 @@
       <c r="I4" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="20" t="s">
-        <v>211</v>
-      </c>
-      <c r="K4" s="21" t="s">
+      <c r="J4" s="66" t="s">
+        <v>210</v>
+      </c>
+      <c r="K4" s="20" t="s">
         <v>20</v>
       </c>
       <c r="L4" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="M4" s="22"/>
-      <c r="N4" s="22"/>
-      <c r="O4" s="33" t="s">
-        <v>202</v>
-      </c>
-      <c r="P4" s="34" t="s">
+      <c r="M4" s="21"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="32" t="s">
+        <v>201</v>
+      </c>
+      <c r="P4" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="Q4" s="35">
+      <c r="Q4" s="34">
         <v>6</v>
       </c>
-      <c r="R4" s="36" t="s">
+      <c r="R4" s="35" t="s">
+        <v>182</v>
+      </c>
+      <c r="S4" s="34" t="s">
         <v>183</v>
       </c>
-      <c r="S4" s="35" t="s">
+      <c r="T4" s="37" t="s">
         <v>184</v>
       </c>
-      <c r="T4" s="38" t="s">
+      <c r="U4" s="34" t="s">
         <v>185</v>
-      </c>
-      <c r="U4" s="35" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15">
@@ -1652,8 +1671,8 @@
       </c>
       <c r="E5" s="16"/>
       <c r="F5" s="18"/>
-      <c r="G5" s="26" t="s">
-        <v>210</v>
+      <c r="G5" s="25" t="s">
+        <v>209</v>
       </c>
       <c r="H5" s="18">
         <v>3</v>
@@ -1661,37 +1680,37 @@
       <c r="I5" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="J5" s="20" t="s">
-        <v>212</v>
-      </c>
-      <c r="K5" s="21" t="s">
+      <c r="J5" s="66" t="s">
+        <v>211</v>
+      </c>
+      <c r="K5" s="20" t="s">
         <v>20</v>
       </c>
       <c r="L5" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="M5" s="22"/>
-      <c r="N5" s="22"/>
-      <c r="O5" s="33" t="s">
-        <v>202</v>
-      </c>
-      <c r="P5" s="34" t="s">
+      <c r="M5" s="21"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="32" t="s">
+        <v>201</v>
+      </c>
+      <c r="P5" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="Q5" s="35">
+      <c r="Q5" s="34">
         <v>6</v>
       </c>
-      <c r="R5" s="36" t="s">
+      <c r="R5" s="35" t="s">
+        <v>182</v>
+      </c>
+      <c r="S5" s="34" t="s">
         <v>183</v>
       </c>
-      <c r="S5" s="35" t="s">
-        <v>184</v>
-      </c>
-      <c r="T5" s="38" t="s">
-        <v>187</v>
-      </c>
-      <c r="U5" s="35" t="s">
+      <c r="T5" s="37" t="s">
         <v>186</v>
+      </c>
+      <c r="U5" s="34" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="15">
@@ -1707,10 +1726,10 @@
       <c r="D6" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="E6" s="39"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="26" t="s">
-        <v>204</v>
+      <c r="E6" s="38"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="25" t="s">
+        <v>203</v>
       </c>
       <c r="H6" s="18">
         <v>4</v>
@@ -1718,10 +1737,10 @@
       <c r="I6" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="J6" s="41" t="s">
-        <v>205</v>
-      </c>
-      <c r="K6" s="21" t="s">
+      <c r="J6" s="67" t="s">
+        <v>204</v>
+      </c>
+      <c r="K6" s="20" t="s">
         <v>19</v>
       </c>
       <c r="L6" s="19" t="s">
@@ -1729,23 +1748,23 @@
       </c>
       <c r="M6" s="8"/>
       <c r="N6" s="8"/>
-      <c r="O6" s="40"/>
-      <c r="P6" s="34" t="s">
+      <c r="O6" s="39"/>
+      <c r="P6" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="Q6" s="35">
+      <c r="Q6" s="34">
         <v>7</v>
       </c>
-      <c r="R6" s="36" t="s">
+      <c r="R6" s="35" t="s">
         <v>137</v>
       </c>
-      <c r="S6" s="35" t="s">
+      <c r="S6" s="34" t="s">
         <v>138</v>
       </c>
-      <c r="T6" s="37" t="s">
+      <c r="T6" s="36" t="s">
         <v>141</v>
       </c>
-      <c r="U6" s="35" t="s">
+      <c r="U6" s="34" t="s">
         <v>140</v>
       </c>
     </row>
@@ -1762,10 +1781,10 @@
       <c r="D7" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="E7" s="39"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="26" t="s">
-        <v>143</v>
+      <c r="E7" s="38"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="25" t="s">
+        <v>221</v>
       </c>
       <c r="H7" s="18">
         <v>5</v>
@@ -1773,10 +1792,10 @@
       <c r="I7" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="J7" s="41" t="s">
-        <v>213</v>
-      </c>
-      <c r="K7" s="21" t="s">
+      <c r="J7" s="67" t="s">
+        <v>212</v>
+      </c>
+      <c r="K7" s="20" t="s">
         <v>20</v>
       </c>
       <c r="L7" s="19" t="s">
@@ -1786,26 +1805,26 @@
       <c r="N7" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="O7" s="40" t="s">
-        <v>144</v>
-      </c>
-      <c r="P7" s="34" t="s">
+      <c r="O7" s="39" t="s">
+        <v>143</v>
+      </c>
+      <c r="P7" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="Q7" s="35">
+      <c r="Q7" s="34">
         <v>6</v>
       </c>
-      <c r="R7" s="36" t="s">
-        <v>183</v>
-      </c>
-      <c r="S7" s="35" t="s">
+      <c r="R7" s="35" t="s">
+        <v>182</v>
+      </c>
+      <c r="S7" s="34" t="s">
+        <v>187</v>
+      </c>
+      <c r="T7" s="41" t="s">
         <v>188</v>
       </c>
-      <c r="T7" s="42" t="s">
+      <c r="U7" s="34" t="s">
         <v>189</v>
-      </c>
-      <c r="U7" s="35" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="15">
@@ -1821,10 +1840,10 @@
       <c r="D8" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="E8" s="39"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="26" t="s">
-        <v>214</v>
+      <c r="E8" s="38"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="25" t="s">
+        <v>213</v>
       </c>
       <c r="H8" s="18">
         <v>6</v>
@@ -1832,10 +1851,10 @@
       <c r="I8" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="J8" s="41" t="s">
-        <v>215</v>
-      </c>
-      <c r="K8" s="21" t="s">
+      <c r="J8" s="67" t="s">
+        <v>214</v>
+      </c>
+      <c r="K8" s="20" t="s">
         <v>20</v>
       </c>
       <c r="L8" s="19" t="s">
@@ -1845,26 +1864,26 @@
       <c r="N8" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="O8" s="40" t="s">
+      <c r="O8" s="39" t="s">
         <v>142</v>
       </c>
-      <c r="P8" s="34" t="s">
+      <c r="P8" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="Q8" s="35">
+      <c r="Q8" s="34">
         <v>6</v>
       </c>
-      <c r="R8" s="36" t="s">
-        <v>183</v>
-      </c>
-      <c r="S8" s="35" t="s">
-        <v>188</v>
-      </c>
-      <c r="T8" s="42" t="s">
-        <v>191</v>
-      </c>
-      <c r="U8" s="35" t="s">
+      <c r="R8" s="35" t="s">
+        <v>182</v>
+      </c>
+      <c r="S8" s="34" t="s">
+        <v>187</v>
+      </c>
+      <c r="T8" s="41" t="s">
         <v>190</v>
+      </c>
+      <c r="U8" s="34" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="15">
@@ -1880,12 +1899,12 @@
       <c r="D9" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="E9" s="39" t="s">
+      <c r="E9" s="38" t="s">
         <v>124</v>
       </c>
-      <c r="F9" s="40"/>
-      <c r="G9" s="26" t="s">
-        <v>145</v>
+      <c r="F9" s="39"/>
+      <c r="G9" s="25" t="s">
+        <v>144</v>
       </c>
       <c r="H9" s="18">
         <v>7</v>
@@ -1893,10 +1912,10 @@
       <c r="I9" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="J9" s="41" t="s">
-        <v>166</v>
-      </c>
-      <c r="K9" s="21" t="s">
+      <c r="J9" s="67" t="s">
+        <v>165</v>
+      </c>
+      <c r="K9" s="20" t="s">
         <v>19</v>
       </c>
       <c r="L9" s="19" t="s">
@@ -1904,23 +1923,23 @@
       </c>
       <c r="M9" s="8"/>
       <c r="N9" s="8"/>
-      <c r="O9" s="40"/>
-      <c r="P9" s="34" t="s">
+      <c r="O9" s="39"/>
+      <c r="P9" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="Q9" s="35">
+      <c r="Q9" s="34">
         <v>7</v>
       </c>
-      <c r="R9" s="36" t="s">
+      <c r="R9" s="35" t="s">
         <v>137</v>
       </c>
-      <c r="S9" s="35" t="s">
+      <c r="S9" s="34" t="s">
         <v>138</v>
       </c>
-      <c r="T9" s="37" t="s">
-        <v>146</v>
-      </c>
-      <c r="U9" s="35" t="s">
+      <c r="T9" s="36" t="s">
+        <v>145</v>
+      </c>
+      <c r="U9" s="34" t="s">
         <v>140</v>
       </c>
     </row>
@@ -1935,12 +1954,12 @@
         <v>138</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>162</v>
-      </c>
-      <c r="E10" s="39"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="26" t="s">
-        <v>147</v>
+        <v>161</v>
+      </c>
+      <c r="E10" s="38"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="25" t="s">
+        <v>146</v>
       </c>
       <c r="H10" s="18">
         <v>8</v>
@@ -1948,10 +1967,10 @@
       <c r="I10" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="J10" s="20" t="s">
-        <v>177</v>
-      </c>
-      <c r="K10" s="21" t="s">
+      <c r="J10" s="66" t="s">
+        <v>176</v>
+      </c>
+      <c r="K10" s="20" t="s">
         <v>20</v>
       </c>
       <c r="L10" s="19" t="s">
@@ -1959,26 +1978,26 @@
       </c>
       <c r="M10" s="8"/>
       <c r="N10" s="8"/>
-      <c r="O10" s="40" t="s">
-        <v>202</v>
-      </c>
-      <c r="P10" s="34" t="s">
+      <c r="O10" s="39" t="s">
+        <v>201</v>
+      </c>
+      <c r="P10" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="Q10" s="35">
+      <c r="Q10" s="34">
         <v>6</v>
       </c>
-      <c r="R10" s="36" t="s">
+      <c r="R10" s="35" t="s">
+        <v>182</v>
+      </c>
+      <c r="S10" s="34" t="s">
         <v>183</v>
       </c>
-      <c r="S10" s="35" t="s">
-        <v>184</v>
-      </c>
-      <c r="T10" s="38" t="s">
-        <v>193</v>
-      </c>
-      <c r="U10" s="35" t="s">
-        <v>186</v>
+      <c r="T10" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="U10" s="34" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="15">
@@ -1992,12 +2011,12 @@
         <v>138</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>162</v>
-      </c>
-      <c r="E11" s="39"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="26" t="s">
-        <v>148</v>
+        <v>161</v>
+      </c>
+      <c r="E11" s="38"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="25" t="s">
+        <v>147</v>
       </c>
       <c r="H11" s="18">
         <v>9</v>
@@ -2005,10 +2024,10 @@
       <c r="I11" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="J11" s="41" t="s">
-        <v>216</v>
-      </c>
-      <c r="K11" s="21" t="s">
+      <c r="J11" s="67" t="s">
+        <v>215</v>
+      </c>
+      <c r="K11" s="20" t="s">
         <v>20</v>
       </c>
       <c r="L11" s="19" t="s">
@@ -2018,26 +2037,26 @@
       <c r="N11" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="O11" s="40" t="s">
-        <v>149</v>
-      </c>
-      <c r="P11" s="34" t="s">
+      <c r="O11" s="39" t="s">
+        <v>148</v>
+      </c>
+      <c r="P11" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="Q11" s="35">
+      <c r="Q11" s="34">
         <v>6</v>
       </c>
-      <c r="R11" s="36" t="s">
-        <v>183</v>
-      </c>
-      <c r="S11" s="35" t="s">
-        <v>188</v>
-      </c>
-      <c r="T11" s="42" t="s">
-        <v>196</v>
-      </c>
-      <c r="U11" s="35" t="s">
-        <v>190</v>
+      <c r="R11" s="35" t="s">
+        <v>182</v>
+      </c>
+      <c r="S11" s="34" t="s">
+        <v>187</v>
+      </c>
+      <c r="T11" s="41" t="s">
+        <v>195</v>
+      </c>
+      <c r="U11" s="34" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="15">
@@ -2051,14 +2070,14 @@
         <v>138</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>162</v>
-      </c>
-      <c r="E12" s="39" t="s">
+        <v>161</v>
+      </c>
+      <c r="E12" s="38" t="s">
         <v>124</v>
       </c>
-      <c r="F12" s="40"/>
-      <c r="G12" s="26" t="s">
-        <v>169</v>
+      <c r="F12" s="39"/>
+      <c r="G12" s="25" t="s">
+        <v>168</v>
       </c>
       <c r="H12" s="18">
         <v>10</v>
@@ -2066,10 +2085,10 @@
       <c r="I12" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="J12" s="41" t="s">
-        <v>178</v>
-      </c>
-      <c r="K12" s="21" t="s">
+      <c r="J12" s="67" t="s">
+        <v>177</v>
+      </c>
+      <c r="K12" s="20" t="s">
         <v>20</v>
       </c>
       <c r="L12" s="19" t="s">
@@ -2077,23 +2096,23 @@
       </c>
       <c r="M12" s="8"/>
       <c r="N12" s="8"/>
-      <c r="O12" s="40"/>
-      <c r="P12" s="34" t="s">
+      <c r="O12" s="39"/>
+      <c r="P12" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="Q12" s="35">
+      <c r="Q12" s="34">
         <v>7</v>
       </c>
-      <c r="R12" s="36" t="s">
+      <c r="R12" s="35" t="s">
         <v>137</v>
       </c>
-      <c r="S12" s="35" t="s">
+      <c r="S12" s="34" t="s">
         <v>138</v>
       </c>
-      <c r="T12" s="37" t="s">
-        <v>182</v>
-      </c>
-      <c r="U12" s="35" t="s">
+      <c r="T12" s="36" t="s">
+        <v>181</v>
+      </c>
+      <c r="U12" s="34" t="s">
         <v>140</v>
       </c>
     </row>
@@ -2108,12 +2127,12 @@
         <v>138</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>150</v>
-      </c>
-      <c r="E13" s="39"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="26" t="s">
-        <v>150</v>
+        <v>149</v>
+      </c>
+      <c r="E13" s="38"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="25" t="s">
+        <v>149</v>
       </c>
       <c r="H13" s="18">
         <v>11</v>
@@ -2121,10 +2140,10 @@
       <c r="I13" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="J13" s="20" t="s">
-        <v>179</v>
-      </c>
-      <c r="K13" s="21" t="s">
+      <c r="J13" s="66" t="s">
+        <v>178</v>
+      </c>
+      <c r="K13" s="20" t="s">
         <v>20</v>
       </c>
       <c r="L13" s="19" t="s">
@@ -2132,26 +2151,26 @@
       </c>
       <c r="M13" s="8"/>
       <c r="N13" s="8"/>
-      <c r="O13" s="40" t="s">
-        <v>202</v>
-      </c>
-      <c r="P13" s="34" t="s">
+      <c r="O13" s="39" t="s">
+        <v>201</v>
+      </c>
+      <c r="P13" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="Q13" s="35">
+      <c r="Q13" s="34">
         <v>6</v>
       </c>
-      <c r="R13" s="36" t="s">
+      <c r="R13" s="35" t="s">
+        <v>182</v>
+      </c>
+      <c r="S13" s="34" t="s">
         <v>183</v>
       </c>
-      <c r="S13" s="35" t="s">
-        <v>184</v>
-      </c>
-      <c r="T13" s="38" t="s">
-        <v>194</v>
-      </c>
-      <c r="U13" s="35" t="s">
-        <v>186</v>
+      <c r="T13" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="U13" s="34" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="15">
@@ -2165,12 +2184,12 @@
         <v>138</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>150</v>
-      </c>
-      <c r="E14" s="39"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="26" t="s">
-        <v>152</v>
+        <v>149</v>
+      </c>
+      <c r="E14" s="38"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="25" t="s">
+        <v>151</v>
       </c>
       <c r="H14" s="18">
         <v>12</v>
@@ -2178,10 +2197,10 @@
       <c r="I14" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J14" s="41" t="s">
-        <v>206</v>
-      </c>
-      <c r="K14" s="21" t="s">
+      <c r="J14" s="67" t="s">
+        <v>205</v>
+      </c>
+      <c r="K14" s="20" t="s">
         <v>19</v>
       </c>
       <c r="L14" s="6" t="s">
@@ -2189,23 +2208,23 @@
       </c>
       <c r="M14" s="8"/>
       <c r="N14" s="8"/>
-      <c r="O14" s="40"/>
-      <c r="P14" s="34" t="s">
+      <c r="O14" s="39"/>
+      <c r="P14" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="Q14" s="35">
+      <c r="Q14" s="34">
         <v>7</v>
       </c>
-      <c r="R14" s="36" t="s">
+      <c r="R14" s="35" t="s">
         <v>137</v>
       </c>
-      <c r="S14" s="35" t="s">
+      <c r="S14" s="34" t="s">
         <v>138</v>
       </c>
-      <c r="T14" s="37" t="s">
-        <v>151</v>
-      </c>
-      <c r="U14" s="35" t="s">
+      <c r="T14" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="U14" s="34" t="s">
         <v>140</v>
       </c>
     </row>
@@ -2220,11 +2239,11 @@
         <v>138</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>150</v>
-      </c>
-      <c r="E15" s="39"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="E15" s="38"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="25" t="s">
         <v>126</v>
       </c>
       <c r="H15" s="18">
@@ -2233,10 +2252,10 @@
       <c r="I15" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J15" s="41" t="s">
-        <v>217</v>
-      </c>
-      <c r="K15" s="21" t="s">
+      <c r="J15" s="67" t="s">
+        <v>216</v>
+      </c>
+      <c r="K15" s="20" t="s">
         <v>19</v>
       </c>
       <c r="L15" s="6" t="s">
@@ -2244,23 +2263,23 @@
       </c>
       <c r="M15" s="8"/>
       <c r="N15" s="8"/>
-      <c r="O15" s="40"/>
-      <c r="P15" s="34" t="s">
+      <c r="O15" s="39"/>
+      <c r="P15" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="Q15" s="35">
+      <c r="Q15" s="34">
         <v>7</v>
       </c>
-      <c r="R15" s="36" t="s">
+      <c r="R15" s="35" t="s">
         <v>137</v>
       </c>
-      <c r="S15" s="35" t="s">
+      <c r="S15" s="34" t="s">
         <v>138</v>
       </c>
-      <c r="T15" s="37" t="s">
+      <c r="T15" s="36" t="s">
         <v>128</v>
       </c>
-      <c r="U15" s="35" t="s">
+      <c r="U15" s="34" t="s">
         <v>140</v>
       </c>
     </row>
@@ -2275,12 +2294,12 @@
         <v>138</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>150</v>
-      </c>
-      <c r="E16" s="39"/>
-      <c r="F16" s="40"/>
-      <c r="G16" s="26" t="s">
-        <v>153</v>
+        <v>149</v>
+      </c>
+      <c r="E16" s="38"/>
+      <c r="F16" s="39"/>
+      <c r="G16" s="25" t="s">
+        <v>152</v>
       </c>
       <c r="H16" s="18">
         <v>14</v>
@@ -2288,10 +2307,10 @@
       <c r="I16" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J16" s="41" t="s">
-        <v>180</v>
-      </c>
-      <c r="K16" s="21" t="s">
+      <c r="J16" s="67" t="s">
+        <v>179</v>
+      </c>
+      <c r="K16" s="20" t="s">
         <v>20</v>
       </c>
       <c r="L16" s="6" t="s">
@@ -2301,26 +2320,26 @@
       <c r="N16" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="O16" s="40" t="s">
-        <v>154</v>
-      </c>
-      <c r="P16" s="43" t="s">
+      <c r="O16" s="39" t="s">
+        <v>153</v>
+      </c>
+      <c r="P16" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="Q16" s="35">
+      <c r="Q16" s="34">
         <v>6</v>
       </c>
-      <c r="R16" s="36" t="s">
-        <v>183</v>
-      </c>
-      <c r="S16" s="35" t="s">
-        <v>188</v>
-      </c>
-      <c r="T16" s="42" t="s">
-        <v>195</v>
-      </c>
-      <c r="U16" s="35" t="s">
-        <v>190</v>
+      <c r="R16" s="35" t="s">
+        <v>182</v>
+      </c>
+      <c r="S16" s="34" t="s">
+        <v>187</v>
+      </c>
+      <c r="T16" s="41" t="s">
+        <v>194</v>
+      </c>
+      <c r="U16" s="34" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="15">
@@ -2334,11 +2353,11 @@
         <v>138</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>150</v>
-      </c>
-      <c r="E17" s="39"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="E17" s="38"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="25" t="s">
         <v>122</v>
       </c>
       <c r="H17" s="18">
@@ -2347,10 +2366,10 @@
       <c r="I17" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J17" s="41" t="s">
-        <v>167</v>
-      </c>
-      <c r="K17" s="21" t="s">
+      <c r="J17" s="67" t="s">
+        <v>166</v>
+      </c>
+      <c r="K17" s="20" t="s">
         <v>19</v>
       </c>
       <c r="L17" s="6" t="s">
@@ -2358,23 +2377,23 @@
       </c>
       <c r="M17" s="8"/>
       <c r="N17" s="8"/>
-      <c r="O17" s="40"/>
-      <c r="P17" s="43" t="s">
+      <c r="O17" s="39"/>
+      <c r="P17" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="Q17" s="35">
+      <c r="Q17" s="34">
         <v>7</v>
       </c>
-      <c r="R17" s="36" t="s">
+      <c r="R17" s="35" t="s">
         <v>137</v>
       </c>
-      <c r="S17" s="35" t="s">
+      <c r="S17" s="34" t="s">
         <v>138</v>
       </c>
-      <c r="T17" s="37" t="s">
+      <c r="T17" s="36" t="s">
         <v>122</v>
       </c>
-      <c r="U17" s="35" t="s">
+      <c r="U17" s="34" t="s">
         <v>140</v>
       </c>
     </row>
@@ -2389,14 +2408,14 @@
         <v>138</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>150</v>
-      </c>
-      <c r="E18" s="39" t="s">
+        <v>149</v>
+      </c>
+      <c r="E18" s="38" t="s">
         <v>124</v>
       </c>
-      <c r="F18" s="40"/>
-      <c r="G18" s="26" t="s">
-        <v>155</v>
+      <c r="F18" s="39"/>
+      <c r="G18" s="25" t="s">
+        <v>154</v>
       </c>
       <c r="H18" s="18">
         <v>16</v>
@@ -2404,10 +2423,10 @@
       <c r="I18" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J18" s="41" t="s">
-        <v>168</v>
-      </c>
-      <c r="K18" s="21" t="s">
+      <c r="J18" s="67" t="s">
+        <v>167</v>
+      </c>
+      <c r="K18" s="20" t="s">
         <v>19</v>
       </c>
       <c r="L18" s="6" t="s">
@@ -2415,23 +2434,23 @@
       </c>
       <c r="M18" s="8"/>
       <c r="N18" s="8"/>
-      <c r="O18" s="40"/>
-      <c r="P18" s="43" t="s">
+      <c r="O18" s="39"/>
+      <c r="P18" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="Q18" s="35">
+      <c r="Q18" s="34">
         <v>7</v>
       </c>
-      <c r="R18" s="36" t="s">
+      <c r="R18" s="35" t="s">
         <v>137</v>
       </c>
-      <c r="S18" s="35" t="s">
+      <c r="S18" s="34" t="s">
         <v>138</v>
       </c>
-      <c r="T18" s="37" t="s">
-        <v>155</v>
-      </c>
-      <c r="U18" s="35" t="s">
+      <c r="T18" s="36" t="s">
+        <v>154</v>
+      </c>
+      <c r="U18" s="34" t="s">
         <v>140</v>
       </c>
     </row>
@@ -2446,11 +2465,11 @@
         <v>138</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E19" s="39"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="26" t="s">
+        <v>206</v>
+      </c>
+      <c r="E19" s="38"/>
+      <c r="F19" s="39"/>
+      <c r="G19" s="25" t="s">
         <v>127</v>
       </c>
       <c r="H19" s="18">
@@ -2459,10 +2478,10 @@
       <c r="I19" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J19" s="41" t="s">
-        <v>170</v>
-      </c>
-      <c r="K19" s="21" t="s">
+      <c r="J19" s="67" t="s">
+        <v>169</v>
+      </c>
+      <c r="K19" s="20" t="s">
         <v>19</v>
       </c>
       <c r="L19" s="6" t="s">
@@ -2470,23 +2489,23 @@
       </c>
       <c r="M19" s="8"/>
       <c r="N19" s="8"/>
-      <c r="O19" s="40"/>
-      <c r="P19" s="43" t="s">
+      <c r="O19" s="39"/>
+      <c r="P19" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="Q19" s="35">
+      <c r="Q19" s="34">
         <v>7</v>
       </c>
-      <c r="R19" s="36" t="s">
+      <c r="R19" s="35" t="s">
         <v>137</v>
       </c>
-      <c r="S19" s="35" t="s">
+      <c r="S19" s="34" t="s">
         <v>138</v>
       </c>
-      <c r="T19" s="37" t="s">
-        <v>156</v>
-      </c>
-      <c r="U19" s="35" t="s">
+      <c r="T19" s="36" t="s">
+        <v>155</v>
+      </c>
+      <c r="U19" s="34" t="s">
         <v>140</v>
       </c>
     </row>
@@ -2501,11 +2520,11 @@
         <v>138</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E20" s="39"/>
-      <c r="F20" s="40"/>
-      <c r="G20" s="26" t="s">
+        <v>206</v>
+      </c>
+      <c r="E20" s="38"/>
+      <c r="F20" s="39"/>
+      <c r="G20" s="25" t="s">
         <v>129</v>
       </c>
       <c r="H20" s="18">
@@ -2514,10 +2533,10 @@
       <c r="I20" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J20" s="41" t="s">
-        <v>208</v>
-      </c>
-      <c r="K20" s="21" t="s">
+      <c r="J20" s="67" t="s">
+        <v>207</v>
+      </c>
+      <c r="K20" s="20" t="s">
         <v>20</v>
       </c>
       <c r="L20" s="6" t="s">
@@ -2525,23 +2544,23 @@
       </c>
       <c r="M20" s="8"/>
       <c r="N20" s="8"/>
-      <c r="O20" s="40"/>
-      <c r="P20" s="43" t="s">
+      <c r="O20" s="39"/>
+      <c r="P20" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="Q20" s="35">
+      <c r="Q20" s="34">
         <v>7</v>
       </c>
-      <c r="R20" s="36" t="s">
+      <c r="R20" s="35" t="s">
         <v>137</v>
       </c>
-      <c r="S20" s="35" t="s">
+      <c r="S20" s="34" t="s">
         <v>138</v>
       </c>
-      <c r="T20" s="37" t="s">
+      <c r="T20" s="36" t="s">
         <v>129</v>
       </c>
-      <c r="U20" s="35" t="s">
+      <c r="U20" s="34" t="s">
         <v>140</v>
       </c>
     </row>
@@ -2556,12 +2575,12 @@
         <v>138</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E21" s="39"/>
-      <c r="F21" s="40"/>
-      <c r="G21" s="26" t="s">
-        <v>181</v>
+        <v>206</v>
+      </c>
+      <c r="E21" s="38"/>
+      <c r="F21" s="39"/>
+      <c r="G21" s="25" t="s">
+        <v>180</v>
       </c>
       <c r="H21" s="18">
         <v>19</v>
@@ -2569,10 +2588,10 @@
       <c r="I21" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J21" s="41" t="s">
-        <v>209</v>
-      </c>
-      <c r="K21" s="21" t="s">
+      <c r="J21" s="67" t="s">
+        <v>208</v>
+      </c>
+      <c r="K21" s="20" t="s">
         <v>19</v>
       </c>
       <c r="L21" s="6" t="s">
@@ -2582,26 +2601,26 @@
       <c r="N21" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="O21" s="40" t="s">
-        <v>199</v>
-      </c>
-      <c r="P21" s="43" t="s">
+      <c r="O21" s="39" t="s">
+        <v>198</v>
+      </c>
+      <c r="P21" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="Q21" s="35">
+      <c r="Q21" s="34">
         <v>6</v>
       </c>
-      <c r="R21" s="36" t="s">
-        <v>183</v>
-      </c>
-      <c r="S21" s="35" t="s">
-        <v>188</v>
-      </c>
-      <c r="T21" s="42" t="s">
-        <v>192</v>
-      </c>
-      <c r="U21" s="35" t="s">
-        <v>190</v>
+      <c r="R21" s="35" t="s">
+        <v>182</v>
+      </c>
+      <c r="S21" s="34" t="s">
+        <v>187</v>
+      </c>
+      <c r="T21" s="41" t="s">
+        <v>191</v>
+      </c>
+      <c r="U21" s="34" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="22" spans="1:21" ht="15">
@@ -2615,11 +2634,11 @@
         <v>138</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E22" s="39"/>
-      <c r="F22" s="40"/>
-      <c r="G22" s="26" t="s">
+        <v>206</v>
+      </c>
+      <c r="E22" s="38"/>
+      <c r="F22" s="39"/>
+      <c r="G22" s="25" t="s">
         <v>130</v>
       </c>
       <c r="H22" s="18">
@@ -2628,10 +2647,10 @@
       <c r="I22" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J22" s="41" t="s">
-        <v>218</v>
-      </c>
-      <c r="K22" s="21" t="s">
+      <c r="J22" s="67" t="s">
+        <v>217</v>
+      </c>
+      <c r="K22" s="20" t="s">
         <v>19</v>
       </c>
       <c r="L22" s="6" t="s">
@@ -2639,23 +2658,23 @@
       </c>
       <c r="M22" s="8"/>
       <c r="N22" s="8"/>
-      <c r="O22" s="40"/>
-      <c r="P22" s="43" t="s">
+      <c r="O22" s="39"/>
+      <c r="P22" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="Q22" s="35">
+      <c r="Q22" s="34">
         <v>7</v>
       </c>
-      <c r="R22" s="36" t="s">
+      <c r="R22" s="35" t="s">
         <v>137</v>
       </c>
-      <c r="S22" s="35" t="s">
+      <c r="S22" s="34" t="s">
         <v>138</v>
       </c>
-      <c r="T22" s="37" t="s">
-        <v>157</v>
-      </c>
-      <c r="U22" s="35" t="s">
+      <c r="T22" s="36" t="s">
+        <v>156</v>
+      </c>
+      <c r="U22" s="34" t="s">
         <v>140</v>
       </c>
     </row>
@@ -2670,11 +2689,11 @@
         <v>138</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E23" s="39"/>
-      <c r="F23" s="40"/>
-      <c r="G23" s="26" t="s">
+        <v>206</v>
+      </c>
+      <c r="E23" s="38"/>
+      <c r="F23" s="39"/>
+      <c r="G23" s="25" t="s">
         <v>131</v>
       </c>
       <c r="H23" s="18">
@@ -2683,10 +2702,10 @@
       <c r="I23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J23" s="41" t="s">
-        <v>171</v>
-      </c>
-      <c r="K23" s="21" t="s">
+      <c r="J23" s="67" t="s">
+        <v>170</v>
+      </c>
+      <c r="K23" s="20" t="s">
         <v>19</v>
       </c>
       <c r="L23" s="6" t="s">
@@ -2694,23 +2713,23 @@
       </c>
       <c r="M23" s="8"/>
       <c r="N23" s="8"/>
-      <c r="O23" s="40"/>
-      <c r="P23" s="43" t="s">
+      <c r="O23" s="39"/>
+      <c r="P23" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="Q23" s="35">
+      <c r="Q23" s="34">
         <v>7</v>
       </c>
-      <c r="R23" s="36" t="s">
+      <c r="R23" s="35" t="s">
         <v>137</v>
       </c>
-      <c r="S23" s="35" t="s">
+      <c r="S23" s="34" t="s">
         <v>138</v>
       </c>
-      <c r="T23" s="37" t="s">
-        <v>158</v>
-      </c>
-      <c r="U23" s="35" t="s">
+      <c r="T23" s="36" t="s">
+        <v>157</v>
+      </c>
+      <c r="U23" s="34" t="s">
         <v>140</v>
       </c>
     </row>
@@ -2725,12 +2744,12 @@
         <v>138</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E24" s="39"/>
-      <c r="F24" s="40"/>
-      <c r="G24" s="26" t="s">
-        <v>159</v>
+        <v>206</v>
+      </c>
+      <c r="E24" s="38"/>
+      <c r="F24" s="39"/>
+      <c r="G24" s="25" t="s">
+        <v>158</v>
       </c>
       <c r="H24" s="18">
         <v>22</v>
@@ -2738,10 +2757,10 @@
       <c r="I24" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J24" s="41" t="s">
-        <v>172</v>
-      </c>
-      <c r="K24" s="21" t="s">
+      <c r="J24" s="67" t="s">
+        <v>171</v>
+      </c>
+      <c r="K24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="L24" s="6" t="s">
@@ -2749,23 +2768,23 @@
       </c>
       <c r="M24" s="8"/>
       <c r="N24" s="8"/>
-      <c r="O24" s="40"/>
-      <c r="P24" s="43" t="s">
+      <c r="O24" s="39"/>
+      <c r="P24" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="Q24" s="35">
+      <c r="Q24" s="34">
         <v>7</v>
       </c>
-      <c r="R24" s="36" t="s">
+      <c r="R24" s="35" t="s">
         <v>137</v>
       </c>
-      <c r="S24" s="35" t="s">
+      <c r="S24" s="34" t="s">
         <v>138</v>
       </c>
-      <c r="T24" s="37" t="s">
-        <v>159</v>
-      </c>
-      <c r="U24" s="35" t="s">
+      <c r="T24" s="36" t="s">
+        <v>158</v>
+      </c>
+      <c r="U24" s="34" t="s">
         <v>140</v>
       </c>
     </row>
@@ -2780,11 +2799,11 @@
         <v>138</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E25" s="39"/>
-      <c r="F25" s="40"/>
-      <c r="G25" s="26" t="s">
+        <v>206</v>
+      </c>
+      <c r="E25" s="38"/>
+      <c r="F25" s="39"/>
+      <c r="G25" s="25" t="s">
         <v>132</v>
       </c>
       <c r="H25" s="18">
@@ -2793,10 +2812,10 @@
       <c r="I25" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J25" s="41" t="s">
-        <v>173</v>
-      </c>
-      <c r="K25" s="21" t="s">
+      <c r="J25" s="67" t="s">
+        <v>172</v>
+      </c>
+      <c r="K25" s="20" t="s">
         <v>19</v>
       </c>
       <c r="L25" s="6" t="s">
@@ -2804,23 +2823,23 @@
       </c>
       <c r="M25" s="8"/>
       <c r="N25" s="8"/>
-      <c r="O25" s="40"/>
-      <c r="P25" s="43" t="s">
+      <c r="O25" s="39"/>
+      <c r="P25" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="Q25" s="35">
+      <c r="Q25" s="34">
         <v>7</v>
       </c>
-      <c r="R25" s="36" t="s">
+      <c r="R25" s="35" t="s">
         <v>137</v>
       </c>
-      <c r="S25" s="35" t="s">
+      <c r="S25" s="34" t="s">
         <v>138</v>
       </c>
-      <c r="T25" s="37" t="s">
+      <c r="T25" s="36" t="s">
         <v>132</v>
       </c>
-      <c r="U25" s="35" t="s">
+      <c r="U25" s="34" t="s">
         <v>140</v>
       </c>
     </row>
@@ -2835,14 +2854,14 @@
         <v>138</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E26" s="39" t="s">
+        <v>206</v>
+      </c>
+      <c r="E26" s="38" t="s">
         <v>124</v>
       </c>
-      <c r="F26" s="40"/>
-      <c r="G26" s="26" t="s">
-        <v>219</v>
+      <c r="F26" s="39"/>
+      <c r="G26" s="25" t="s">
+        <v>218</v>
       </c>
       <c r="H26" s="18">
         <v>24</v>
@@ -2850,10 +2869,10 @@
       <c r="I26" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J26" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="K26" s="21" t="s">
+      <c r="J26" s="67" t="s">
+        <v>173</v>
+      </c>
+      <c r="K26" s="20" t="s">
         <v>19</v>
       </c>
       <c r="L26" s="6" t="s">
@@ -2861,23 +2880,23 @@
       </c>
       <c r="M26" s="8"/>
       <c r="N26" s="8"/>
-      <c r="O26" s="40"/>
-      <c r="P26" s="43" t="s">
+      <c r="O26" s="39"/>
+      <c r="P26" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="Q26" s="35">
+      <c r="Q26" s="34">
         <v>7</v>
       </c>
-      <c r="R26" s="36" t="s">
+      <c r="R26" s="35" t="s">
         <v>137</v>
       </c>
-      <c r="S26" s="35" t="s">
+      <c r="S26" s="34" t="s">
         <v>138</v>
       </c>
-      <c r="T26" s="37" t="s">
+      <c r="T26" s="36" t="s">
         <v>133</v>
       </c>
-      <c r="U26" s="35" t="s">
+      <c r="U26" s="34" t="s">
         <v>140</v>
       </c>
     </row>
@@ -2891,12 +2910,12 @@
       <c r="C27" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="D27" s="44" t="s">
-        <v>163</v>
-      </c>
-      <c r="E27" s="39"/>
-      <c r="F27" s="40"/>
-      <c r="G27" s="26" t="s">
+      <c r="D27" s="43" t="s">
+        <v>162</v>
+      </c>
+      <c r="E27" s="38"/>
+      <c r="F27" s="39"/>
+      <c r="G27" s="25" t="s">
         <v>134</v>
       </c>
       <c r="H27" s="18">
@@ -2905,10 +2924,10 @@
       <c r="I27" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J27" s="41" t="s">
-        <v>220</v>
-      </c>
-      <c r="K27" s="21" t="s">
+      <c r="J27" s="67" t="s">
+        <v>219</v>
+      </c>
+      <c r="K27" s="20" t="s">
         <v>19</v>
       </c>
       <c r="L27" s="6" t="s">
@@ -2916,23 +2935,23 @@
       </c>
       <c r="M27" s="8"/>
       <c r="N27" s="8"/>
-      <c r="O27" s="40"/>
-      <c r="P27" s="43" t="s">
+      <c r="O27" s="39"/>
+      <c r="P27" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="Q27" s="35">
+      <c r="Q27" s="34">
         <v>7</v>
       </c>
-      <c r="R27" s="36" t="s">
+      <c r="R27" s="35" t="s">
         <v>137</v>
       </c>
-      <c r="S27" s="35" t="s">
+      <c r="S27" s="34" t="s">
         <v>138</v>
       </c>
-      <c r="T27" s="37" t="s">
+      <c r="T27" s="36" t="s">
         <v>134</v>
       </c>
-      <c r="U27" s="35" t="s">
+      <c r="U27" s="34" t="s">
         <v>140</v>
       </c>
     </row>
@@ -2946,13 +2965,13 @@
       <c r="C28" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="D28" s="44" t="s">
-        <v>163</v>
-      </c>
-      <c r="E28" s="39"/>
-      <c r="F28" s="40"/>
-      <c r="G28" s="26" t="s">
-        <v>161</v>
+      <c r="D28" s="43" t="s">
+        <v>162</v>
+      </c>
+      <c r="E28" s="38"/>
+      <c r="F28" s="39"/>
+      <c r="G28" s="25" t="s">
+        <v>160</v>
       </c>
       <c r="H28" s="18">
         <v>26</v>
@@ -2960,10 +2979,10 @@
       <c r="I28" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J28" s="41" t="s">
-        <v>221</v>
-      </c>
-      <c r="K28" s="21" t="s">
+      <c r="J28" s="67" t="s">
+        <v>220</v>
+      </c>
+      <c r="K28" s="20" t="s">
         <v>19</v>
       </c>
       <c r="L28" s="6" t="s">
@@ -2971,23 +2990,23 @@
       </c>
       <c r="M28" s="8"/>
       <c r="N28" s="8"/>
-      <c r="O28" s="40"/>
-      <c r="P28" s="43" t="s">
+      <c r="O28" s="39"/>
+      <c r="P28" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="Q28" s="35">
+      <c r="Q28" s="34">
         <v>7</v>
       </c>
-      <c r="R28" s="36" t="s">
+      <c r="R28" s="35" t="s">
         <v>137</v>
       </c>
-      <c r="S28" s="35" t="s">
+      <c r="S28" s="34" t="s">
         <v>138</v>
       </c>
-      <c r="T28" s="37" t="s">
-        <v>160</v>
-      </c>
-      <c r="U28" s="35" t="s">
+      <c r="T28" s="36" t="s">
+        <v>159</v>
+      </c>
+      <c r="U28" s="34" t="s">
         <v>140</v>
       </c>
     </row>
@@ -3001,12 +3020,12 @@
       <c r="C29" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="D29" s="44" t="s">
-        <v>164</v>
-      </c>
-      <c r="E29" s="39"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="26" t="s">
+      <c r="D29" s="43" t="s">
+        <v>163</v>
+      </c>
+      <c r="E29" s="38"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="25" t="s">
         <v>10</v>
       </c>
       <c r="H29" s="18">
@@ -3015,10 +3034,10 @@
       <c r="I29" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J29" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="K29" s="21" t="s">
+      <c r="J29" s="67" t="s">
+        <v>174</v>
+      </c>
+      <c r="K29" s="20" t="s">
         <v>20</v>
       </c>
       <c r="L29" s="6" t="s">
@@ -3026,15 +3045,15 @@
       </c>
       <c r="M29" s="8"/>
       <c r="N29" s="8"/>
-      <c r="O29" s="40"/>
-      <c r="P29" s="43" t="s">
+      <c r="O29" s="39"/>
+      <c r="P29" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="Q29" s="35"/>
-      <c r="R29" s="36"/>
-      <c r="S29" s="35"/>
-      <c r="T29" s="37"/>
-      <c r="U29" s="35"/>
+      <c r="Q29" s="34"/>
+      <c r="R29" s="35"/>
+      <c r="S29" s="34"/>
+      <c r="T29" s="36"/>
+      <c r="U29" s="34"/>
     </row>
     <row r="30" spans="1:21" ht="15">
       <c r="A30" s="15" t="s">
@@ -3046,12 +3065,12 @@
       <c r="C30" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="D30" s="44" t="s">
-        <v>164</v>
-      </c>
-      <c r="E30" s="39"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="26" t="s">
+      <c r="D30" s="43" t="s">
+        <v>163</v>
+      </c>
+      <c r="E30" s="38"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="25" t="s">
         <v>123</v>
       </c>
       <c r="H30" s="18">
@@ -3060,10 +3079,10 @@
       <c r="I30" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J30" s="41" t="s">
-        <v>176</v>
-      </c>
-      <c r="K30" s="21" t="s">
+      <c r="J30" s="67" t="s">
+        <v>175</v>
+      </c>
+      <c r="K30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="L30" s="6" t="s">
@@ -3073,26 +3092,26 @@
       <c r="N30" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="O30" s="40" t="s">
-        <v>200</v>
-      </c>
-      <c r="P30" s="43" t="s">
+      <c r="O30" s="39" t="s">
+        <v>199</v>
+      </c>
+      <c r="P30" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="Q30" s="35">
+      <c r="Q30" s="34">
         <v>6</v>
       </c>
-      <c r="R30" s="36" t="s">
-        <v>183</v>
-      </c>
-      <c r="S30" s="35" t="s">
-        <v>188</v>
-      </c>
-      <c r="T30" s="42" t="s">
-        <v>197</v>
-      </c>
-      <c r="U30" s="35" t="s">
-        <v>190</v>
+      <c r="R30" s="35" t="s">
+        <v>182</v>
+      </c>
+      <c r="S30" s="34" t="s">
+        <v>187</v>
+      </c>
+      <c r="T30" s="41" t="s">
+        <v>196</v>
+      </c>
+      <c r="U30" s="34" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="31" spans="1:21" ht="15">
@@ -3105,13 +3124,13 @@
       <c r="C31" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="D31" s="44" t="s">
-        <v>165</v>
-      </c>
-      <c r="E31" s="39"/>
-      <c r="F31" s="40"/>
-      <c r="G31" s="44" t="s">
-        <v>165</v>
+      <c r="D31" s="43" t="s">
+        <v>164</v>
+      </c>
+      <c r="E31" s="38"/>
+      <c r="F31" s="39"/>
+      <c r="G31" s="43" t="s">
+        <v>164</v>
       </c>
       <c r="H31" s="18">
         <v>29</v>
@@ -3119,7 +3138,7 @@
       <c r="I31" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J31" s="41"/>
+      <c r="J31" s="40"/>
       <c r="K31" s="7" t="s">
         <v>19</v>
       </c>
@@ -3128,26 +3147,26 @@
       <c r="N31" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="O31" s="40" t="s">
-        <v>198</v>
-      </c>
-      <c r="P31" s="43" t="s">
+      <c r="O31" s="39" t="s">
+        <v>197</v>
+      </c>
+      <c r="P31" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="Q31" s="35">
+      <c r="Q31" s="34">
         <v>6</v>
       </c>
-      <c r="R31" s="36" t="s">
-        <v>183</v>
-      </c>
-      <c r="S31" s="35" t="s">
-        <v>188</v>
-      </c>
-      <c r="T31" s="37" t="s">
-        <v>203</v>
-      </c>
-      <c r="U31" s="35" t="s">
-        <v>190</v>
+      <c r="R31" s="35" t="s">
+        <v>182</v>
+      </c>
+      <c r="S31" s="34" t="s">
+        <v>187</v>
+      </c>
+      <c r="T31" s="36" t="s">
+        <v>202</v>
+      </c>
+      <c r="U31" s="34" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="32" spans="1:21" ht="15">
@@ -3165,12 +3184,12 @@
       <c r="M32" s="8"/>
       <c r="N32" s="8"/>
       <c r="O32" s="9"/>
-      <c r="P32" s="25"/>
-      <c r="Q32" s="28"/>
-      <c r="R32" s="32"/>
-      <c r="S32" s="28"/>
-      <c r="T32" s="30"/>
-      <c r="U32" s="28"/>
+      <c r="P32" s="24"/>
+      <c r="Q32" s="27"/>
+      <c r="R32" s="31"/>
+      <c r="S32" s="27"/>
+      <c r="T32" s="29"/>
+      <c r="U32" s="27"/>
     </row>
     <row r="33" spans="1:21" ht="15">
       <c r="A33" s="15"/>
@@ -3179,7 +3198,7 @@
       <c r="D33" s="12"/>
       <c r="E33" s="10"/>
       <c r="F33" s="9"/>
-      <c r="H33" s="25"/>
+      <c r="H33" s="24"/>
       <c r="I33" s="5"/>
       <c r="J33" s="14"/>
       <c r="K33" s="7"/>
@@ -3187,12 +3206,12 @@
       <c r="M33" s="8"/>
       <c r="N33" s="8"/>
       <c r="O33" s="9"/>
-      <c r="P33" s="25"/>
-      <c r="Q33" s="28"/>
-      <c r="R33" s="32"/>
-      <c r="S33" s="28"/>
-      <c r="T33" s="30"/>
-      <c r="U33" s="28"/>
+      <c r="P33" s="24"/>
+      <c r="Q33" s="27"/>
+      <c r="R33" s="31"/>
+      <c r="S33" s="27"/>
+      <c r="T33" s="29"/>
+      <c r="U33" s="27"/>
     </row>
     <row r="34" spans="1:21" ht="15">
       <c r="A34" s="15"/>
@@ -3201,7 +3220,7 @@
       <c r="D34" s="12"/>
       <c r="E34" s="10"/>
       <c r="F34" s="9"/>
-      <c r="H34" s="25"/>
+      <c r="H34" s="24"/>
       <c r="I34" s="5"/>
       <c r="J34" s="14"/>
       <c r="K34" s="7"/>
@@ -3209,12 +3228,12 @@
       <c r="M34" s="8"/>
       <c r="N34" s="8"/>
       <c r="O34" s="9"/>
-      <c r="P34" s="25"/>
-      <c r="Q34" s="28"/>
-      <c r="R34" s="29"/>
-      <c r="S34" s="28"/>
-      <c r="T34" s="30"/>
-      <c r="U34" s="28"/>
+      <c r="P34" s="24"/>
+      <c r="Q34" s="27"/>
+      <c r="R34" s="28"/>
+      <c r="S34" s="27"/>
+      <c r="T34" s="29"/>
+      <c r="U34" s="27"/>
     </row>
     <row r="35" spans="1:21" ht="15">
       <c r="A35" s="15"/>
@@ -3232,12 +3251,12 @@
       <c r="M35" s="8"/>
       <c r="N35" s="8"/>
       <c r="O35" s="9"/>
-      <c r="P35" s="25"/>
-      <c r="Q35" s="28"/>
-      <c r="R35" s="29"/>
-      <c r="S35" s="28"/>
-      <c r="T35" s="30"/>
-      <c r="U35" s="28"/>
+      <c r="P35" s="24"/>
+      <c r="Q35" s="27"/>
+      <c r="R35" s="28"/>
+      <c r="S35" s="27"/>
+      <c r="T35" s="29"/>
+      <c r="U35" s="27"/>
     </row>
     <row r="36" spans="1:21" ht="15">
       <c r="A36" s="15"/>
@@ -3247,7 +3266,7 @@
       <c r="E36" s="10"/>
       <c r="F36" s="9"/>
       <c r="G36" s="13"/>
-      <c r="H36" s="25"/>
+      <c r="H36" s="24"/>
       <c r="I36" s="5"/>
       <c r="J36" s="14"/>
       <c r="K36" s="7"/>
@@ -3255,12 +3274,12 @@
       <c r="M36" s="8"/>
       <c r="N36" s="8"/>
       <c r="O36" s="9"/>
-      <c r="P36" s="25"/>
-      <c r="Q36" s="28"/>
-      <c r="R36" s="29"/>
-      <c r="S36" s="28"/>
-      <c r="T36" s="30"/>
-      <c r="U36" s="28"/>
+      <c r="P36" s="24"/>
+      <c r="Q36" s="27"/>
+      <c r="R36" s="28"/>
+      <c r="S36" s="27"/>
+      <c r="T36" s="29"/>
+      <c r="U36" s="27"/>
     </row>
     <row r="37" spans="1:21" ht="15">
       <c r="A37" s="15"/>
@@ -3278,12 +3297,12 @@
       <c r="M37" s="8"/>
       <c r="N37" s="8"/>
       <c r="O37" s="9"/>
-      <c r="P37" s="25"/>
-      <c r="Q37" s="28"/>
-      <c r="R37" s="29"/>
-      <c r="S37" s="28"/>
-      <c r="T37" s="30"/>
-      <c r="U37" s="28"/>
+      <c r="P37" s="24"/>
+      <c r="Q37" s="27"/>
+      <c r="R37" s="28"/>
+      <c r="S37" s="27"/>
+      <c r="T37" s="29"/>
+      <c r="U37" s="27"/>
     </row>
     <row r="38" spans="1:21" ht="15">
       <c r="A38" s="15"/>
@@ -3293,7 +3312,7 @@
       <c r="E38" s="10"/>
       <c r="F38" s="9"/>
       <c r="G38" s="13"/>
-      <c r="H38" s="25"/>
+      <c r="H38" s="24"/>
       <c r="I38" s="5"/>
       <c r="J38" s="14"/>
       <c r="K38" s="7"/>
@@ -3301,12 +3320,12 @@
       <c r="M38" s="8"/>
       <c r="N38" s="8"/>
       <c r="O38" s="9"/>
-      <c r="P38" s="25"/>
-      <c r="Q38" s="28"/>
-      <c r="R38" s="29"/>
-      <c r="S38" s="28"/>
-      <c r="T38" s="30"/>
-      <c r="U38" s="28"/>
+      <c r="P38" s="24"/>
+      <c r="Q38" s="27"/>
+      <c r="R38" s="28"/>
+      <c r="S38" s="27"/>
+      <c r="T38" s="29"/>
+      <c r="U38" s="27"/>
     </row>
     <row r="39" spans="1:21" ht="15">
       <c r="A39" s="15"/>
@@ -3316,7 +3335,7 @@
       <c r="E39" s="10"/>
       <c r="F39" s="9"/>
       <c r="G39" s="13"/>
-      <c r="H39" s="25"/>
+      <c r="H39" s="24"/>
       <c r="I39" s="5"/>
       <c r="J39" s="14"/>
       <c r="K39" s="7"/>
@@ -3324,12 +3343,12 @@
       <c r="M39" s="8"/>
       <c r="N39" s="8"/>
       <c r="O39" s="9"/>
-      <c r="P39" s="25"/>
-      <c r="Q39" s="28"/>
-      <c r="R39" s="29"/>
-      <c r="S39" s="28"/>
-      <c r="T39" s="30"/>
-      <c r="U39" s="28"/>
+      <c r="P39" s="24"/>
+      <c r="Q39" s="27"/>
+      <c r="R39" s="28"/>
+      <c r="S39" s="27"/>
+      <c r="T39" s="29"/>
+      <c r="U39" s="27"/>
     </row>
     <row r="40" spans="1:21" ht="15">
       <c r="A40" s="15"/>
@@ -3347,12 +3366,12 @@
       <c r="M40" s="8"/>
       <c r="N40" s="8"/>
       <c r="O40" s="9"/>
-      <c r="P40" s="25"/>
-      <c r="Q40" s="28"/>
-      <c r="R40" s="29"/>
-      <c r="S40" s="28"/>
-      <c r="T40" s="30"/>
-      <c r="U40" s="28"/>
+      <c r="P40" s="24"/>
+      <c r="Q40" s="27"/>
+      <c r="R40" s="28"/>
+      <c r="S40" s="27"/>
+      <c r="T40" s="29"/>
+      <c r="U40" s="27"/>
     </row>
     <row r="41" spans="1:21" ht="15">
       <c r="A41" s="4"/>
@@ -3370,12 +3389,12 @@
       <c r="M41" s="8"/>
       <c r="N41" s="8"/>
       <c r="O41" s="9"/>
-      <c r="P41" s="25"/>
-      <c r="Q41" s="28"/>
-      <c r="R41" s="29"/>
-      <c r="S41" s="28"/>
-      <c r="T41" s="30"/>
-      <c r="U41" s="28"/>
+      <c r="P41" s="24"/>
+      <c r="Q41" s="27"/>
+      <c r="R41" s="28"/>
+      <c r="S41" s="27"/>
+      <c r="T41" s="29"/>
+      <c r="U41" s="27"/>
     </row>
     <row r="42" spans="1:21" ht="15">
       <c r="A42" s="4"/>
@@ -3393,12 +3412,12 @@
       <c r="M42" s="8"/>
       <c r="N42" s="8"/>
       <c r="O42" s="9"/>
-      <c r="P42" s="25"/>
-      <c r="Q42" s="28"/>
-      <c r="R42" s="29"/>
-      <c r="S42" s="28"/>
-      <c r="T42" s="30"/>
-      <c r="U42" s="28"/>
+      <c r="P42" s="24"/>
+      <c r="Q42" s="27"/>
+      <c r="R42" s="28"/>
+      <c r="S42" s="27"/>
+      <c r="T42" s="29"/>
+      <c r="U42" s="27"/>
     </row>
     <row r="43" spans="1:21" ht="15">
       <c r="A43" s="4"/>
@@ -3416,12 +3435,12 @@
       <c r="M43" s="8"/>
       <c r="N43" s="8"/>
       <c r="O43" s="9"/>
-      <c r="P43" s="25"/>
-      <c r="Q43" s="28"/>
-      <c r="R43" s="29"/>
-      <c r="S43" s="28"/>
-      <c r="T43" s="30"/>
-      <c r="U43" s="28"/>
+      <c r="P43" s="24"/>
+      <c r="Q43" s="27"/>
+      <c r="R43" s="28"/>
+      <c r="S43" s="27"/>
+      <c r="T43" s="29"/>
+      <c r="U43" s="27"/>
     </row>
     <row r="44" spans="1:21" ht="15">
       <c r="A44" s="4"/>
@@ -3439,12 +3458,12 @@
       <c r="M44" s="8"/>
       <c r="N44" s="8"/>
       <c r="O44" s="9"/>
-      <c r="P44" s="25"/>
-      <c r="Q44" s="28"/>
-      <c r="R44" s="29"/>
-      <c r="S44" s="28"/>
-      <c r="T44" s="30"/>
-      <c r="U44" s="28"/>
+      <c r="P44" s="24"/>
+      <c r="Q44" s="27"/>
+      <c r="R44" s="28"/>
+      <c r="S44" s="27"/>
+      <c r="T44" s="29"/>
+      <c r="U44" s="27"/>
     </row>
     <row r="45" spans="1:21" ht="15">
       <c r="A45" s="4"/>
@@ -3462,12 +3481,12 @@
       <c r="M45" s="8"/>
       <c r="N45" s="8"/>
       <c r="O45" s="9"/>
-      <c r="P45" s="25"/>
-      <c r="Q45" s="28"/>
-      <c r="R45" s="29"/>
-      <c r="S45" s="28"/>
-      <c r="T45" s="30"/>
-      <c r="U45" s="28"/>
+      <c r="P45" s="24"/>
+      <c r="Q45" s="27"/>
+      <c r="R45" s="28"/>
+      <c r="S45" s="27"/>
+      <c r="T45" s="29"/>
+      <c r="U45" s="27"/>
     </row>
     <row r="46" spans="1:21" ht="15">
       <c r="A46" s="4"/>
@@ -3485,12 +3504,12 @@
       <c r="M46" s="8"/>
       <c r="N46" s="8"/>
       <c r="O46" s="9"/>
-      <c r="P46" s="25"/>
-      <c r="Q46" s="28"/>
-      <c r="R46" s="29"/>
-      <c r="S46" s="28"/>
-      <c r="T46" s="30"/>
-      <c r="U46" s="28"/>
+      <c r="P46" s="24"/>
+      <c r="Q46" s="27"/>
+      <c r="R46" s="28"/>
+      <c r="S46" s="27"/>
+      <c r="T46" s="29"/>
+      <c r="U46" s="27"/>
     </row>
     <row r="47" spans="1:21" ht="15">
       <c r="A47" s="4"/>
@@ -3508,12 +3527,12 @@
       <c r="M47" s="8"/>
       <c r="N47" s="8"/>
       <c r="O47" s="9"/>
-      <c r="P47" s="25"/>
-      <c r="Q47" s="28"/>
-      <c r="R47" s="29"/>
-      <c r="S47" s="28"/>
-      <c r="T47" s="30"/>
-      <c r="U47" s="28"/>
+      <c r="P47" s="24"/>
+      <c r="Q47" s="27"/>
+      <c r="R47" s="28"/>
+      <c r="S47" s="27"/>
+      <c r="T47" s="29"/>
+      <c r="U47" s="27"/>
     </row>
     <row r="48" spans="1:21" ht="15">
       <c r="A48" s="4"/>
@@ -3531,12 +3550,12 @@
       <c r="M48" s="8"/>
       <c r="N48" s="8"/>
       <c r="O48" s="9"/>
-      <c r="P48" s="25"/>
-      <c r="Q48" s="28"/>
-      <c r="R48" s="29"/>
-      <c r="S48" s="28"/>
-      <c r="T48" s="30"/>
-      <c r="U48" s="28"/>
+      <c r="P48" s="24"/>
+      <c r="Q48" s="27"/>
+      <c r="R48" s="28"/>
+      <c r="S48" s="27"/>
+      <c r="T48" s="29"/>
+      <c r="U48" s="27"/>
     </row>
     <row r="49" spans="1:21" ht="15">
       <c r="A49" s="4"/>
@@ -3554,12 +3573,12 @@
       <c r="M49" s="8"/>
       <c r="N49" s="8"/>
       <c r="O49" s="9"/>
-      <c r="P49" s="25"/>
-      <c r="Q49" s="28"/>
-      <c r="R49" s="29"/>
-      <c r="S49" s="28"/>
-      <c r="T49" s="30"/>
-      <c r="U49" s="28"/>
+      <c r="P49" s="24"/>
+      <c r="Q49" s="27"/>
+      <c r="R49" s="28"/>
+      <c r="S49" s="27"/>
+      <c r="T49" s="29"/>
+      <c r="U49" s="27"/>
     </row>
     <row r="50" spans="1:21" ht="15">
       <c r="A50" s="4"/>
@@ -3577,12 +3596,12 @@
       <c r="M50" s="8"/>
       <c r="N50" s="8"/>
       <c r="O50" s="9"/>
-      <c r="P50" s="25"/>
-      <c r="Q50" s="28"/>
-      <c r="R50" s="29"/>
-      <c r="S50" s="28"/>
-      <c r="T50" s="30"/>
-      <c r="U50" s="28"/>
+      <c r="P50" s="24"/>
+      <c r="Q50" s="27"/>
+      <c r="R50" s="28"/>
+      <c r="S50" s="27"/>
+      <c r="T50" s="29"/>
+      <c r="U50" s="27"/>
     </row>
     <row r="51" spans="1:21" ht="15">
       <c r="A51" s="4"/>
@@ -3600,12 +3619,12 @@
       <c r="M51" s="8"/>
       <c r="N51" s="8"/>
       <c r="O51" s="9"/>
-      <c r="P51" s="25"/>
-      <c r="Q51" s="28"/>
-      <c r="R51" s="29"/>
-      <c r="S51" s="28"/>
-      <c r="T51" s="30"/>
-      <c r="U51" s="28"/>
+      <c r="P51" s="24"/>
+      <c r="Q51" s="27"/>
+      <c r="R51" s="28"/>
+      <c r="S51" s="27"/>
+      <c r="T51" s="29"/>
+      <c r="U51" s="27"/>
     </row>
     <row r="52" spans="1:21" ht="15">
       <c r="A52" s="4"/>
@@ -3623,12 +3642,12 @@
       <c r="M52" s="8"/>
       <c r="N52" s="8"/>
       <c r="O52" s="9"/>
-      <c r="P52" s="25"/>
-      <c r="Q52" s="28"/>
-      <c r="R52" s="29"/>
-      <c r="S52" s="28"/>
-      <c r="T52" s="30"/>
-      <c r="U52" s="28"/>
+      <c r="P52" s="24"/>
+      <c r="Q52" s="27"/>
+      <c r="R52" s="28"/>
+      <c r="S52" s="27"/>
+      <c r="T52" s="29"/>
+      <c r="U52" s="27"/>
     </row>
     <row r="53" spans="1:21" ht="15">
       <c r="A53" s="4"/>
@@ -3646,12 +3665,12 @@
       <c r="M53" s="8"/>
       <c r="N53" s="8"/>
       <c r="O53" s="9"/>
-      <c r="P53" s="25"/>
-      <c r="Q53" s="28"/>
-      <c r="R53" s="29"/>
-      <c r="S53" s="28"/>
-      <c r="T53" s="30"/>
-      <c r="U53" s="28"/>
+      <c r="P53" s="24"/>
+      <c r="Q53" s="27"/>
+      <c r="R53" s="28"/>
+      <c r="S53" s="27"/>
+      <c r="T53" s="29"/>
+      <c r="U53" s="27"/>
     </row>
     <row r="54" spans="1:21" ht="15">
       <c r="A54" s="4"/>
@@ -3669,12 +3688,12 @@
       <c r="M54" s="8"/>
       <c r="N54" s="8"/>
       <c r="O54" s="9"/>
-      <c r="P54" s="25"/>
-      <c r="Q54" s="28"/>
-      <c r="R54" s="29"/>
-      <c r="S54" s="28"/>
-      <c r="T54" s="30"/>
-      <c r="U54" s="28"/>
+      <c r="P54" s="24"/>
+      <c r="Q54" s="27"/>
+      <c r="R54" s="28"/>
+      <c r="S54" s="27"/>
+      <c r="T54" s="29"/>
+      <c r="U54" s="27"/>
     </row>
     <row r="55" spans="1:21" ht="15">
       <c r="A55" s="4"/>
@@ -3692,12 +3711,12 @@
       <c r="M55" s="8"/>
       <c r="N55" s="8"/>
       <c r="O55" s="9"/>
-      <c r="P55" s="25"/>
-      <c r="Q55" s="28"/>
-      <c r="R55" s="29"/>
-      <c r="S55" s="28"/>
-      <c r="T55" s="30"/>
-      <c r="U55" s="28"/>
+      <c r="P55" s="24"/>
+      <c r="Q55" s="27"/>
+      <c r="R55" s="28"/>
+      <c r="S55" s="27"/>
+      <c r="T55" s="29"/>
+      <c r="U55" s="27"/>
     </row>
     <row r="56" spans="1:21" ht="15">
       <c r="A56" s="4"/>
@@ -3715,12 +3734,12 @@
       <c r="M56" s="8"/>
       <c r="N56" s="8"/>
       <c r="O56" s="9"/>
-      <c r="P56" s="25"/>
-      <c r="Q56" s="28"/>
-      <c r="R56" s="29"/>
-      <c r="S56" s="28"/>
-      <c r="T56" s="30"/>
-      <c r="U56" s="28"/>
+      <c r="P56" s="24"/>
+      <c r="Q56" s="27"/>
+      <c r="R56" s="28"/>
+      <c r="S56" s="27"/>
+      <c r="T56" s="29"/>
+      <c r="U56" s="27"/>
     </row>
     <row r="57" spans="1:21" ht="15">
       <c r="A57" s="4"/>
@@ -3738,12 +3757,12 @@
       <c r="M57" s="8"/>
       <c r="N57" s="8"/>
       <c r="O57" s="9"/>
-      <c r="P57" s="25"/>
-      <c r="Q57" s="28"/>
-      <c r="R57" s="29"/>
-      <c r="S57" s="28"/>
-      <c r="T57" s="30"/>
-      <c r="U57" s="28"/>
+      <c r="P57" s="24"/>
+      <c r="Q57" s="27"/>
+      <c r="R57" s="28"/>
+      <c r="S57" s="27"/>
+      <c r="T57" s="29"/>
+      <c r="U57" s="27"/>
     </row>
     <row r="58" spans="1:21" ht="15">
       <c r="A58" s="4"/>
@@ -3761,12 +3780,12 @@
       <c r="M58" s="8"/>
       <c r="N58" s="8"/>
       <c r="O58" s="9"/>
-      <c r="P58" s="25"/>
-      <c r="Q58" s="28"/>
-      <c r="R58" s="29"/>
-      <c r="S58" s="28"/>
-      <c r="T58" s="30"/>
-      <c r="U58" s="28"/>
+      <c r="P58" s="24"/>
+      <c r="Q58" s="27"/>
+      <c r="R58" s="28"/>
+      <c r="S58" s="27"/>
+      <c r="T58" s="29"/>
+      <c r="U58" s="27"/>
     </row>
     <row r="59" spans="1:21" ht="15">
       <c r="A59" s="4"/>
@@ -3784,12 +3803,12 @@
       <c r="M59" s="8"/>
       <c r="N59" s="8"/>
       <c r="O59" s="9"/>
-      <c r="P59" s="25"/>
-      <c r="Q59" s="28"/>
-      <c r="R59" s="29"/>
-      <c r="S59" s="28"/>
-      <c r="T59" s="30"/>
-      <c r="U59" s="28"/>
+      <c r="P59" s="24"/>
+      <c r="Q59" s="27"/>
+      <c r="R59" s="28"/>
+      <c r="S59" s="27"/>
+      <c r="T59" s="29"/>
+      <c r="U59" s="27"/>
     </row>
     <row r="60" spans="1:21" ht="15">
       <c r="A60" s="4"/>
@@ -3807,12 +3826,12 @@
       <c r="M60" s="8"/>
       <c r="N60" s="8"/>
       <c r="O60" s="9"/>
-      <c r="P60" s="25"/>
-      <c r="Q60" s="28"/>
-      <c r="R60" s="29"/>
-      <c r="S60" s="28"/>
-      <c r="T60" s="30"/>
-      <c r="U60" s="28"/>
+      <c r="P60" s="24"/>
+      <c r="Q60" s="27"/>
+      <c r="R60" s="28"/>
+      <c r="S60" s="27"/>
+      <c r="T60" s="29"/>
+      <c r="U60" s="27"/>
     </row>
     <row r="61" spans="1:21" ht="15">
       <c r="A61" s="4"/>
@@ -3830,12 +3849,12 @@
       <c r="M61" s="8"/>
       <c r="N61" s="8"/>
       <c r="O61" s="9"/>
-      <c r="P61" s="25"/>
-      <c r="Q61" s="28"/>
-      <c r="R61" s="29"/>
-      <c r="S61" s="28"/>
-      <c r="T61" s="30"/>
-      <c r="U61" s="28"/>
+      <c r="P61" s="24"/>
+      <c r="Q61" s="27"/>
+      <c r="R61" s="28"/>
+      <c r="S61" s="27"/>
+      <c r="T61" s="29"/>
+      <c r="U61" s="27"/>
     </row>
     <row r="62" spans="1:21" ht="15">
       <c r="A62" s="4"/>
@@ -3853,12 +3872,12 @@
       <c r="M62" s="8"/>
       <c r="N62" s="8"/>
       <c r="O62" s="9"/>
-      <c r="P62" s="25"/>
-      <c r="Q62" s="28"/>
-      <c r="R62" s="29"/>
-      <c r="S62" s="28"/>
-      <c r="T62" s="30"/>
-      <c r="U62" s="28"/>
+      <c r="P62" s="24"/>
+      <c r="Q62" s="27"/>
+      <c r="R62" s="28"/>
+      <c r="S62" s="27"/>
+      <c r="T62" s="29"/>
+      <c r="U62" s="27"/>
     </row>
     <row r="63" spans="1:21" ht="15">
       <c r="A63" s="4"/>
@@ -3876,12 +3895,12 @@
       <c r="M63" s="8"/>
       <c r="N63" s="8"/>
       <c r="O63" s="9"/>
-      <c r="P63" s="25"/>
-      <c r="Q63" s="28"/>
-      <c r="R63" s="29"/>
-      <c r="S63" s="28"/>
-      <c r="T63" s="30"/>
-      <c r="U63" s="28"/>
+      <c r="P63" s="24"/>
+      <c r="Q63" s="27"/>
+      <c r="R63" s="28"/>
+      <c r="S63" s="27"/>
+      <c r="T63" s="29"/>
+      <c r="U63" s="27"/>
     </row>
     <row r="64" spans="1:21" ht="15">
       <c r="A64" s="4"/>
@@ -3899,12 +3918,12 @@
       <c r="M64" s="8"/>
       <c r="N64" s="8"/>
       <c r="O64" s="9"/>
-      <c r="P64" s="25"/>
-      <c r="Q64" s="28"/>
-      <c r="R64" s="29"/>
-      <c r="S64" s="28"/>
-      <c r="T64" s="30"/>
-      <c r="U64" s="28"/>
+      <c r="P64" s="24"/>
+      <c r="Q64" s="27"/>
+      <c r="R64" s="28"/>
+      <c r="S64" s="27"/>
+      <c r="T64" s="29"/>
+      <c r="U64" s="27"/>
     </row>
     <row r="65" spans="1:21" ht="15">
       <c r="A65" s="4"/>
@@ -3922,12 +3941,12 @@
       <c r="M65" s="8"/>
       <c r="N65" s="8"/>
       <c r="O65" s="9"/>
-      <c r="P65" s="25"/>
-      <c r="Q65" s="28"/>
-      <c r="R65" s="29"/>
-      <c r="S65" s="28"/>
-      <c r="T65" s="30"/>
-      <c r="U65" s="28"/>
+      <c r="P65" s="24"/>
+      <c r="Q65" s="27"/>
+      <c r="R65" s="28"/>
+      <c r="S65" s="27"/>
+      <c r="T65" s="29"/>
+      <c r="U65" s="27"/>
     </row>
     <row r="66" spans="1:21" ht="15">
       <c r="A66" s="4"/>
@@ -3945,12 +3964,12 @@
       <c r="M66" s="8"/>
       <c r="N66" s="8"/>
       <c r="O66" s="9"/>
-      <c r="P66" s="25"/>
-      <c r="Q66" s="28"/>
-      <c r="R66" s="29"/>
-      <c r="S66" s="28"/>
-      <c r="T66" s="30"/>
-      <c r="U66" s="28"/>
+      <c r="P66" s="24"/>
+      <c r="Q66" s="27"/>
+      <c r="R66" s="28"/>
+      <c r="S66" s="27"/>
+      <c r="T66" s="29"/>
+      <c r="U66" s="27"/>
     </row>
     <row r="67" spans="1:21" ht="15">
       <c r="A67" s="4"/>
@@ -3968,12 +3987,12 @@
       <c r="M67" s="8"/>
       <c r="N67" s="8"/>
       <c r="O67" s="9"/>
-      <c r="P67" s="25"/>
-      <c r="Q67" s="28"/>
-      <c r="R67" s="29"/>
-      <c r="S67" s="28"/>
-      <c r="T67" s="30"/>
-      <c r="U67" s="28"/>
+      <c r="P67" s="24"/>
+      <c r="Q67" s="27"/>
+      <c r="R67" s="28"/>
+      <c r="S67" s="27"/>
+      <c r="T67" s="29"/>
+      <c r="U67" s="27"/>
     </row>
     <row r="68" spans="1:21" ht="15">
       <c r="A68" s="4"/>
@@ -3991,12 +4010,12 @@
       <c r="M68" s="8"/>
       <c r="N68" s="8"/>
       <c r="O68" s="9"/>
-      <c r="P68" s="25"/>
-      <c r="Q68" s="28"/>
-      <c r="R68" s="29"/>
-      <c r="S68" s="28"/>
-      <c r="T68" s="30"/>
-      <c r="U68" s="28"/>
+      <c r="P68" s="24"/>
+      <c r="Q68" s="27"/>
+      <c r="R68" s="28"/>
+      <c r="S68" s="27"/>
+      <c r="T68" s="29"/>
+      <c r="U68" s="27"/>
     </row>
     <row r="69" spans="1:21" ht="15">
       <c r="A69" s="4"/>
@@ -4014,12 +4033,12 @@
       <c r="M69" s="8"/>
       <c r="N69" s="8"/>
       <c r="O69" s="9"/>
-      <c r="P69" s="25"/>
-      <c r="Q69" s="28"/>
-      <c r="R69" s="29"/>
-      <c r="S69" s="28"/>
-      <c r="T69" s="30"/>
-      <c r="U69" s="28"/>
+      <c r="P69" s="24"/>
+      <c r="Q69" s="27"/>
+      <c r="R69" s="28"/>
+      <c r="S69" s="27"/>
+      <c r="T69" s="29"/>
+      <c r="U69" s="27"/>
     </row>
     <row r="70" spans="1:21" ht="15">
       <c r="A70" s="4"/>
@@ -4037,12 +4056,12 @@
       <c r="M70" s="8"/>
       <c r="N70" s="8"/>
       <c r="O70" s="9"/>
-      <c r="P70" s="25"/>
-      <c r="Q70" s="28"/>
-      <c r="R70" s="29"/>
-      <c r="S70" s="28"/>
-      <c r="T70" s="30"/>
-      <c r="U70" s="28"/>
+      <c r="P70" s="24"/>
+      <c r="Q70" s="27"/>
+      <c r="R70" s="28"/>
+      <c r="S70" s="27"/>
+      <c r="T70" s="29"/>
+      <c r="U70" s="27"/>
     </row>
     <row r="71" spans="1:21" ht="15">
       <c r="A71" s="4"/>
@@ -4060,12 +4079,12 @@
       <c r="M71" s="8"/>
       <c r="N71" s="8"/>
       <c r="O71" s="9"/>
-      <c r="P71" s="25"/>
-      <c r="Q71" s="28"/>
-      <c r="R71" s="29"/>
-      <c r="S71" s="28"/>
-      <c r="T71" s="30"/>
-      <c r="U71" s="28"/>
+      <c r="P71" s="24"/>
+      <c r="Q71" s="27"/>
+      <c r="R71" s="28"/>
+      <c r="S71" s="27"/>
+      <c r="T71" s="29"/>
+      <c r="U71" s="27"/>
     </row>
     <row r="72" spans="1:21" ht="15">
       <c r="A72" s="4"/>
@@ -4083,12 +4102,12 @@
       <c r="M72" s="8"/>
       <c r="N72" s="8"/>
       <c r="O72" s="9"/>
-      <c r="P72" s="25"/>
-      <c r="Q72" s="28"/>
-      <c r="R72" s="29"/>
-      <c r="S72" s="28"/>
-      <c r="T72" s="30"/>
-      <c r="U72" s="28"/>
+      <c r="P72" s="24"/>
+      <c r="Q72" s="27"/>
+      <c r="R72" s="28"/>
+      <c r="S72" s="27"/>
+      <c r="T72" s="29"/>
+      <c r="U72" s="27"/>
     </row>
     <row r="73" spans="1:21" ht="15">
       <c r="A73" s="4"/>
@@ -4106,12 +4125,12 @@
       <c r="M73" s="8"/>
       <c r="N73" s="8"/>
       <c r="O73" s="9"/>
-      <c r="P73" s="25"/>
-      <c r="Q73" s="28"/>
-      <c r="R73" s="29"/>
-      <c r="S73" s="28"/>
-      <c r="T73" s="30"/>
-      <c r="U73" s="28"/>
+      <c r="P73" s="24"/>
+      <c r="Q73" s="27"/>
+      <c r="R73" s="28"/>
+      <c r="S73" s="27"/>
+      <c r="T73" s="29"/>
+      <c r="U73" s="27"/>
     </row>
     <row r="74" spans="1:21" ht="15">
       <c r="A74" s="4"/>
@@ -4129,12 +4148,12 @@
       <c r="M74" s="8"/>
       <c r="N74" s="8"/>
       <c r="O74" s="9"/>
-      <c r="P74" s="25"/>
-      <c r="Q74" s="28"/>
-      <c r="R74" s="29"/>
-      <c r="S74" s="28"/>
-      <c r="T74" s="30"/>
-      <c r="U74" s="28"/>
+      <c r="P74" s="24"/>
+      <c r="Q74" s="27"/>
+      <c r="R74" s="28"/>
+      <c r="S74" s="27"/>
+      <c r="T74" s="29"/>
+      <c r="U74" s="27"/>
     </row>
     <row r="75" spans="1:21" ht="15">
       <c r="A75" s="4"/>
@@ -4152,12 +4171,12 @@
       <c r="M75" s="8"/>
       <c r="N75" s="8"/>
       <c r="O75" s="9"/>
-      <c r="P75" s="25"/>
-      <c r="Q75" s="28"/>
-      <c r="R75" s="29"/>
-      <c r="S75" s="28"/>
-      <c r="T75" s="30"/>
-      <c r="U75" s="28"/>
+      <c r="P75" s="24"/>
+      <c r="Q75" s="27"/>
+      <c r="R75" s="28"/>
+      <c r="S75" s="27"/>
+      <c r="T75" s="29"/>
+      <c r="U75" s="27"/>
     </row>
     <row r="76" spans="1:21" ht="15">
       <c r="A76" s="4"/>
@@ -4175,12 +4194,12 @@
       <c r="M76" s="8"/>
       <c r="N76" s="8"/>
       <c r="O76" s="9"/>
-      <c r="P76" s="25"/>
-      <c r="Q76" s="28"/>
-      <c r="R76" s="29"/>
-      <c r="S76" s="28"/>
-      <c r="T76" s="30"/>
-      <c r="U76" s="28"/>
+      <c r="P76" s="24"/>
+      <c r="Q76" s="27"/>
+      <c r="R76" s="28"/>
+      <c r="S76" s="27"/>
+      <c r="T76" s="29"/>
+      <c r="U76" s="27"/>
     </row>
     <row r="77" spans="1:21" ht="15">
       <c r="A77" s="4"/>
@@ -4198,12 +4217,12 @@
       <c r="M77" s="8"/>
       <c r="N77" s="8"/>
       <c r="O77" s="9"/>
-      <c r="P77" s="25"/>
-      <c r="Q77" s="28"/>
-      <c r="R77" s="29"/>
-      <c r="S77" s="28"/>
-      <c r="T77" s="30"/>
-      <c r="U77" s="28"/>
+      <c r="P77" s="24"/>
+      <c r="Q77" s="27"/>
+      <c r="R77" s="28"/>
+      <c r="S77" s="27"/>
+      <c r="T77" s="29"/>
+      <c r="U77" s="27"/>
     </row>
     <row r="78" spans="1:21" ht="15">
       <c r="A78" s="4"/>
@@ -4221,12 +4240,12 @@
       <c r="M78" s="8"/>
       <c r="N78" s="8"/>
       <c r="O78" s="9"/>
-      <c r="P78" s="25"/>
-      <c r="Q78" s="28"/>
-      <c r="R78" s="29"/>
-      <c r="S78" s="28"/>
-      <c r="T78" s="30"/>
-      <c r="U78" s="28"/>
+      <c r="P78" s="24"/>
+      <c r="Q78" s="27"/>
+      <c r="R78" s="28"/>
+      <c r="S78" s="27"/>
+      <c r="T78" s="29"/>
+      <c r="U78" s="27"/>
     </row>
     <row r="79" spans="1:21" ht="15">
       <c r="A79" s="4"/>
@@ -4244,12 +4263,12 @@
       <c r="M79" s="8"/>
       <c r="N79" s="8"/>
       <c r="O79" s="9"/>
-      <c r="P79" s="25"/>
-      <c r="Q79" s="28"/>
-      <c r="R79" s="29"/>
-      <c r="S79" s="28"/>
-      <c r="T79" s="30"/>
-      <c r="U79" s="28"/>
+      <c r="P79" s="24"/>
+      <c r="Q79" s="27"/>
+      <c r="R79" s="28"/>
+      <c r="S79" s="27"/>
+      <c r="T79" s="29"/>
+      <c r="U79" s="27"/>
     </row>
     <row r="80" spans="1:21" ht="15">
       <c r="A80" s="4"/>
@@ -4267,12 +4286,12 @@
       <c r="M80" s="8"/>
       <c r="N80" s="8"/>
       <c r="O80" s="9"/>
-      <c r="P80" s="25"/>
-      <c r="Q80" s="28"/>
-      <c r="R80" s="29"/>
-      <c r="S80" s="28"/>
-      <c r="T80" s="30"/>
-      <c r="U80" s="28"/>
+      <c r="P80" s="24"/>
+      <c r="Q80" s="27"/>
+      <c r="R80" s="28"/>
+      <c r="S80" s="27"/>
+      <c r="T80" s="29"/>
+      <c r="U80" s="27"/>
     </row>
     <row r="81" spans="1:21" ht="15">
       <c r="A81" s="4"/>
@@ -4290,12 +4309,12 @@
       <c r="M81" s="8"/>
       <c r="N81" s="8"/>
       <c r="O81" s="9"/>
-      <c r="P81" s="25"/>
-      <c r="Q81" s="28"/>
-      <c r="R81" s="29"/>
-      <c r="S81" s="28"/>
-      <c r="T81" s="30"/>
-      <c r="U81" s="28"/>
+      <c r="P81" s="24"/>
+      <c r="Q81" s="27"/>
+      <c r="R81" s="28"/>
+      <c r="S81" s="27"/>
+      <c r="T81" s="29"/>
+      <c r="U81" s="27"/>
     </row>
     <row r="83" spans="1:21" hidden="1"/>
     <row r="84" spans="1:21" hidden="1"/>
@@ -4660,12 +4679,6 @@
     <row r="295" hidden="1"/>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4680,8 +4693,15 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">

</xml_diff>